<commit_message>
Working on new analysis scripts
</commit_message>
<xml_diff>
--- a/EMPANADA Data Files Key.xlsx
+++ b/EMPANADA Data Files Key.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
   <si>
     <t>Original File Name:</t>
   </si>
@@ -30,40 +30,82 @@
     <t>Speed:</t>
   </si>
   <si>
+    <t>2018-11-13 07.33.47.mov</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>2018-11-13 07.55.37.mov</t>
+  </si>
+  <si>
+    <t>Day1-Martian-70mms.mov</t>
+  </si>
+  <si>
+    <t>Martian</t>
+  </si>
+  <si>
+    <t>2018-11-13 07.56.49.mov</t>
+  </si>
+  <si>
+    <t>Day1-Martian-210mms.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 07.58.04.mov</t>
+  </si>
+  <si>
+    <t>Day1-Martian-130mms.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 07.59.29.mov</t>
+  </si>
+  <si>
+    <t>Day1-Lunar-70mms.mov</t>
+  </si>
+  <si>
+    <t>Lunar</t>
+  </si>
+  <si>
     <t>2018-11-13 08.00.45.mov</t>
   </si>
   <si>
     <t>Day1-Lunar-210mms.mov</t>
   </si>
   <si>
-    <t>Lunar</t>
-  </si>
-  <si>
-    <t>2018-11-13 07.59.29.mov</t>
-  </si>
-  <si>
-    <t>Day1-Lunar-70mms.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 07.58.04.mov</t>
-  </si>
-  <si>
-    <t>Day1-Martian-130mms.mov</t>
-  </si>
-  <si>
-    <t>Martian</t>
-  </si>
-  <si>
-    <t>2018-11-13 07.56.49.mov</t>
-  </si>
-  <si>
-    <t>Day1-Martian-210mms.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 07.55.37.mov</t>
-  </si>
-  <si>
-    <t>Day1-Martian-70mms.mov</t>
+    <t>2018-11-13 08.03.53.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-70mms-1.mov</t>
+  </si>
+  <si>
+    <t>Micro</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.23.12.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-70mms-2.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.40.00.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-70mms-3.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.14.47.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-90mms-1.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.32.20.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-90mms-2.mov</t>
   </si>
   <si>
     <t>2018-11-13 08.17.18.mov</t>
@@ -72,9 +114,6 @@
     <t>Day1-Micro-110mms-1.mov</t>
   </si>
   <si>
-    <t>Micro</t>
-  </si>
-  <si>
     <t>2018-11-13 08.34.56.mov</t>
   </si>
   <si>
@@ -186,43 +225,7 @@
     <t>2018-11-13 08.33.38.mov</t>
   </si>
   <si>
-    <t>2018-11-13 08.03.53.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-70mms-1.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.23.12.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-70mms-2.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.40.00.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-70mms-3.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.14.47.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-90mms-1.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.32.20.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-90mms-2.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 07.33.47.mov</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Earth</t>
+    <t>Day1-Micro-230mms-2.mov</t>
   </si>
 </sst>
 </file>
@@ -266,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -276,10 +279,11 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -523,7 +527,7 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2">
@@ -531,23 +535,20 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="2">
-        <v>210.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2">
         <v>1.0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2">
         <v>70.0</v>
@@ -555,50 +556,50 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E4" s="2">
-        <v>130.0</v>
+        <v>210.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="2">
         <v>1.0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2">
-        <v>210.0</v>
+        <v>130.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="2">
         <v>1.0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E6" s="2">
         <v>70.0</v>
@@ -606,448 +607,452 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="4">
-        <v>110.0</v>
+      <c r="E7" s="2">
+        <v>210.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="2">
         <v>1.0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E8" s="2">
-        <v>110.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="C9" s="2">
         <v>1.0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E9" s="4">
-        <v>130.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C10" s="2">
         <v>1.0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E10" s="4">
-        <v>130.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C11" s="2">
         <v>1.0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E11" s="2">
-        <v>130.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="C12" s="2">
         <v>1.0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E12" s="4">
-        <v>150.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C13" s="2">
         <v>1.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="2">
-        <v>150.0</v>
+        <v>22</v>
+      </c>
+      <c r="E13" s="4">
+        <v>110.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C14" s="2">
         <v>1.0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="4">
-        <v>150.0</v>
+        <v>22</v>
+      </c>
+      <c r="E14" s="2">
+        <v>110.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C15" s="2">
         <v>1.0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E15" s="4">
-        <v>170.0</v>
+        <v>130.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C16" s="2">
         <v>1.0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="2">
-        <v>170.0</v>
+        <v>22</v>
+      </c>
+      <c r="E16" s="4">
+        <v>130.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C17" s="2">
         <v>1.0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="4">
-        <v>170.0</v>
+        <v>22</v>
+      </c>
+      <c r="E17" s="2">
+        <v>130.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="B18" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C18" s="2">
         <v>1.0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="2">
-        <v>190.0</v>
+        <v>22</v>
+      </c>
+      <c r="E18" s="4">
+        <v>150.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="B19" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C19" s="2">
         <v>1.0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="4">
-        <v>190.0</v>
+        <v>22</v>
+      </c>
+      <c r="E19" s="2">
+        <v>150.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="B20" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="C20" s="2">
         <v>1.0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E20" s="4">
-        <v>210.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="B21" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C21" s="2">
         <v>1.0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E21" s="4">
-        <v>210.0</v>
+        <v>170.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="C22" s="2">
         <v>1.0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E22" s="2">
-        <v>210.0</v>
+        <v>170.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="B23" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="C23" s="2">
         <v>1.0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E23" s="4">
-        <v>210.0</v>
+        <v>170.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="B24" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="C24" s="2">
         <v>1.0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="4">
-        <v>210.0</v>
+        <v>22</v>
+      </c>
+      <c r="E24" s="2">
+        <v>190.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="B25" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="C25" s="2">
         <v>1.0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="2">
-        <v>230.0</v>
+        <v>22</v>
+      </c>
+      <c r="E25" s="4">
+        <v>190.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C26" s="2">
         <v>1.0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E26" s="4">
-        <v>230.0</v>
+        <v>210.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C27" s="2">
         <v>1.0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="2">
-        <v>70.0</v>
+        <v>22</v>
+      </c>
+      <c r="E27" s="4">
+        <v>210.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C28" s="2">
         <v>1.0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="4">
-        <v>70.0</v>
+        <v>22</v>
+      </c>
+      <c r="E28" s="2">
+        <v>210.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C29" s="2">
         <v>1.0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E29" s="4">
-        <v>70.0</v>
+        <v>210.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C30" s="2">
         <v>1.0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="2">
-        <v>90.0</v>
+        <v>22</v>
+      </c>
+      <c r="E30" s="4">
+        <v>210.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C31" s="2">
         <v>1.0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E31" s="4">
-        <v>90.0</v>
+        <v>22</v>
+      </c>
+      <c r="E31" s="2">
+        <v>230.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="C32" s="2">
         <v>1.0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>69</v>
+        <v>22</v>
+      </c>
+      <c r="E32" s="4">
+        <v>230.0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="$A$1:$E$32">
     <sortState ref="A1:E32">
+      <sortCondition ref="E1:E32"/>
+      <sortCondition ref="A1:A32"/>
       <sortCondition ref="B1:B32"/>
-      <sortCondition ref="E1:E32"/>
       <sortCondition ref="D1:D32"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Generated various slip counting graphs based on parameter and ignore questionable data now
</commit_message>
<xml_diff>
--- a/EMPANADA Data Files Key.xlsx
+++ b/EMPANADA Data Files Key.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$E$38</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$Z$999</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
   <si>
     <t>Original File Name:</t>
   </si>
@@ -36,6 +36,9 @@
     <t>Crop end time:</t>
   </si>
   <si>
+    <t>Questionable:</t>
+  </si>
+  <si>
     <t>2018-11-13 08.00.45.mov</t>
   </si>
   <si>
@@ -45,24 +48,12 @@
     <t>Lunar</t>
   </si>
   <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>2018-11-13 07.59.29.mov</t>
   </si>
   <si>
     <t>Day1-Lunar-70mms.mov</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
     <t>2018-11-13 07.58.04.mov</t>
   </si>
   <si>
@@ -72,33 +63,18 @@
     <t>Martian</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>2018-11-13 07.56.49.mov</t>
   </si>
   <si>
     <t>Day1-Martian-210mms.mov</t>
   </si>
   <si>
-    <t>09</t>
-  </si>
-  <si>
     <t>2018-11-13 07.55.37.mov</t>
   </si>
   <si>
     <t>Day1-Martian-70mms.mov</t>
   </si>
   <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>2018-11-13 08.17.18.mov</t>
   </si>
   <si>
@@ -108,30 +84,18 @@
     <t>Micro</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>2018-11-13 08.34.56.mov</t>
   </si>
   <si>
     <t>Day1-Micro-110mms-2.mov</t>
   </si>
   <si>
-    <t>06</t>
-  </si>
-  <si>
     <t>2018-11-13 08.07.49.mov</t>
   </si>
   <si>
     <t>Day1-Micro-130mms-1.mov</t>
   </si>
   <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
     <t>2018-11-13 08.27.10.mov</t>
   </si>
   <si>
@@ -144,19 +108,13 @@
     <t>Day1-Micro-130mms-3.mov</t>
   </si>
   <si>
-    <t>26</t>
-  </si>
-  <si>
     <t>2018-11-13 08.06.30.mov</t>
   </si>
   <si>
     <t>Day1-Micro-150mms-1.mov</t>
   </si>
   <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>Questionable gravity</t>
+    <t>Yes</t>
   </si>
   <si>
     <t>2018-11-13 08.25.45.mov</t>
@@ -183,9 +141,6 @@
     <t>Day1-Micro-170mms-2.mov</t>
   </si>
   <si>
-    <t>22</t>
-  </si>
-  <si>
     <t>2018-11-13 08.45.13.mov</t>
   </si>
   <si>
@@ -198,9 +153,6 @@
     <t>Day1-Micro-190mms-1.mov</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
     <t>2018-11-13 08.36.14.mov</t>
   </si>
   <si>
@@ -237,9 +189,6 @@
     <t>Day1-Micro-210mms-5.mov</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
     <t>2018-11-13 08.16.05.mov</t>
   </si>
   <si>
@@ -258,21 +207,12 @@
     <t>Day1-Micro-70mms-1.mov</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
     <t>2018-11-13 08.23.12.mov</t>
   </si>
   <si>
     <t>Day1-Micro-70mms-2.mov</t>
   </si>
   <si>
-    <t>43</t>
-  </si>
-  <si>
     <t>2018-11-13 08.40.00.mov</t>
   </si>
   <si>
@@ -285,22 +225,16 @@
     <t>Day1-Micro-90mms-1.mov</t>
   </si>
   <si>
-    <t>35</t>
-  </si>
-  <si>
     <t>2018-11-13 08.32.20.mov</t>
   </si>
   <si>
     <t>Day1-Micro-90mms-2.mov</t>
   </si>
   <si>
-    <t>34</t>
-  </si>
-  <si>
     <t>2018-11-14 08.49.53.mov</t>
   </si>
   <si>
-    <t>2018-11-14 08.52.29.mov</t>
+    <t>2018-11-14 08.48.47.mov</t>
   </si>
   <si>
     <t>2018-11-14 08.44.42.mov</t>
@@ -310,9 +244,6 @@
   </si>
   <si>
     <t>2018-11-14 08.42.19.mov</t>
-  </si>
-  <si>
-    <t>2018-11-14 08.48.47.mov</t>
   </si>
   <si>
     <t>2018-11-13 07.33.47.mov</t>
@@ -345,18 +276,12 @@
     </font>
     <font/>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6B8AF"/>
-        <bgColor rgb="FFE6B8AF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -365,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -376,10 +301,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -598,8 +520,14 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.86"/>
-    <col customWidth="1" min="2" max="2" width="26.71"/>
+    <col customWidth="1" min="1" max="1" width="22.0"/>
+    <col customWidth="1" min="2" max="2" width="24.0"/>
+    <col customWidth="1" min="3" max="3" width="7.86"/>
+    <col customWidth="1" min="4" max="4" width="10.86"/>
+    <col customWidth="1" min="5" max="5" width="10.14"/>
+    <col customWidth="1" min="6" max="6" width="18.86"/>
+    <col customWidth="1" min="7" max="7" width="17.14"/>
+    <col customWidth="1" min="8" max="8" width="16.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -624,730 +552,739 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2">
         <v>1.0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
         <v>210.0</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>11</v>
+      <c r="F2" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>20.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="C3" s="2">
         <v>1.0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2">
         <v>70.0</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>15</v>
+      <c r="F3" s="4">
+        <v>15.0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>44.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2">
         <v>1.0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2">
         <v>130.0</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>20</v>
+      <c r="F4" s="4">
+        <v>11.0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>27.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2">
         <v>1.0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2">
         <v>210.0</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>11</v>
+      <c r="F5" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>20.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2">
         <v>1.0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2">
         <v>70.0</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>27</v>
+      <c r="F6" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>32.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2">
         <v>1.0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="5">
+        <v>22</v>
+      </c>
+      <c r="E7" s="4">
         <v>110.0</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>31</v>
+      <c r="F7" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>30.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2">
         <v>1.0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="2">
+        <v>22</v>
+      </c>
+      <c r="E8" s="4">
         <v>110.0</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>31</v>
+      <c r="F8" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>30.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2">
         <v>1.0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="5">
+        <v>22</v>
+      </c>
+      <c r="E9" s="4">
         <v>130.0</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>38</v>
+      <c r="F9" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>28.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2">
         <v>1.0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="5">
+        <v>22</v>
+      </c>
+      <c r="E10" s="4">
         <v>130.0</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>20</v>
+      <c r="F10" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>27.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2">
         <v>1.0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="2">
+        <v>22</v>
+      </c>
+      <c r="E11" s="4">
         <v>130.0</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>43</v>
+      <c r="F11" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>26.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2">
         <v>1.0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="5">
+        <v>22</v>
+      </c>
+      <c r="E12" s="4">
         <v>150.0</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>47</v>
+      <c r="F12" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>24.0</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C13" s="2">
         <v>1.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="2">
+        <v>22</v>
+      </c>
+      <c r="E13" s="4">
         <v>150.0</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>43</v>
+      <c r="F13" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>26.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C14" s="2">
         <v>1.0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="5">
+        <v>22</v>
+      </c>
+      <c r="E14" s="4">
         <v>150.0</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>46</v>
+      <c r="F14" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>24.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2">
         <v>1.0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="5">
+        <v>22</v>
+      </c>
+      <c r="E15" s="4">
         <v>170.0</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>46</v>
+      <c r="F15" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>24.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C16" s="2">
         <v>1.0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="2">
+        <v>22</v>
+      </c>
+      <c r="E16" s="4">
         <v>170.0</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>56</v>
+      <c r="F16" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>22.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C17" s="2">
         <v>1.0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="5">
+        <v>22</v>
+      </c>
+      <c r="E17" s="4">
         <v>170.0</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>56</v>
+      <c r="F17" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>22.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C18" s="2">
         <v>1.0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="2">
+        <v>22</v>
+      </c>
+      <c r="E18" s="4">
         <v>190.0</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>61</v>
+      <c r="F18" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>21.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C19" s="2">
         <v>1.0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="5">
+        <v>22</v>
+      </c>
+      <c r="E19" s="4">
         <v>190.0</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>61</v>
+      <c r="F19" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>21.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C20" s="2">
         <v>1.0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="5">
+        <v>22</v>
+      </c>
+      <c r="E20" s="4">
         <v>210.0</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>47</v>
+      <c r="F20" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C21" s="2">
         <v>1.0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="5">
+        <v>22</v>
+      </c>
+      <c r="E21" s="4">
         <v>210.0</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>11</v>
+      <c r="F21" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>20.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C22" s="2">
         <v>1.0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="2">
+        <v>22</v>
+      </c>
+      <c r="E22" s="4">
         <v>210.0</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>11</v>
+      <c r="F22" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>20.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C23" s="2">
         <v>1.0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23" s="5">
+        <v>22</v>
+      </c>
+      <c r="E23" s="4">
         <v>210.0</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>11</v>
+      <c r="F23" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>20.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C24" s="2">
         <v>1.0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="5">
+        <v>22</v>
+      </c>
+      <c r="E24" s="4">
         <v>210.0</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>74</v>
+      <c r="F24" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>19.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C25" s="2">
         <v>1.0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="2">
+        <v>22</v>
+      </c>
+      <c r="E25" s="4">
         <v>230.0</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>74</v>
+      <c r="F25" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>19.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C26" s="2">
         <v>1.0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="5">
+        <v>22</v>
+      </c>
+      <c r="E26" s="4">
         <v>230.0</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>74</v>
+      <c r="F26" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>19.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C27" s="2">
         <v>1.0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="2">
+        <v>22</v>
+      </c>
+      <c r="E27" s="4">
         <v>70.0</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>82</v>
+      <c r="F27" s="4">
+        <v>16.0</v>
+      </c>
+      <c r="G27" s="4">
+        <v>42.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C28" s="2">
         <v>1.0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="5">
+        <v>22</v>
+      </c>
+      <c r="E28" s="4">
         <v>70.0</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>47</v>
+      <c r="F28" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G28" s="4">
+        <v>43.0</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C29" s="2">
         <v>1.0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="5">
+        <v>22</v>
+      </c>
+      <c r="E29" s="4">
         <v>70.0</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>82</v>
+      <c r="F29" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G29" s="4">
+        <v>42.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="C30" s="2">
         <v>1.0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="2">
+        <v>22</v>
+      </c>
+      <c r="E30" s="4">
         <v>90.0</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>90</v>
+      <c r="F30" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G30" s="4">
+        <v>35.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C31" s="2">
         <v>1.0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="5">
+        <v>22</v>
+      </c>
+      <c r="E31" s="4">
         <v>90.0</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>47</v>
+      <c r="F31" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>34.0</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="B32" s="3" t="str">
-        <f t="shared" ref="B32:B37" si="1">"Day"&amp;C32&amp;"-"&amp;D32&amp;"-"&amp;E32&amp;"mms.mov"</f>
+        <f t="shared" ref="B32:B36" si="1">"Day"&amp;C32&amp;"-"&amp;D32&amp;"-"&amp;E32&amp;"mms.mov"</f>
         <v>Day2-Lunar-210mms.mov</v>
       </c>
       <c r="C32" s="2">
         <v>2.0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E32" s="2">
         <v>210.0</v>
       </c>
+      <c r="F32" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>19.0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="B33" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1356,16 +1293,22 @@
       <c r="C33" s="2">
         <v>2.0</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="2">
+      <c r="D33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="4">
         <v>70.0</v>
+      </c>
+      <c r="F33" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G33" s="4">
+        <v>42.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="B34" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1375,15 +1318,21 @@
         <v>2.0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E34" s="2">
         <v>130.0</v>
       </c>
+      <c r="F34" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G34" s="4">
+        <v>26.0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="B35" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1393,15 +1342,21 @@
         <v>2.0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E35" s="2">
         <v>210.0</v>
       </c>
+      <c r="F35" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G35" s="4">
+        <v>19.0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B36" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1411,51 +1366,36 @@
         <v>2.0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="5">
+        <v>15</v>
+      </c>
+      <c r="E36" s="4">
         <v>70.0</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G36" s="4">
+        <v>33.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B37" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Day2-Martian-70mms.mov</v>
+        <v>77</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C37" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="5">
-        <v>70.0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$E$38">
-    <sortState ref="A1:E38">
-      <sortCondition ref="B1:B38"/>
-      <sortCondition ref="E1:E38"/>
-      <sortCondition ref="A1:A38"/>
-      <sortCondition ref="D1:D38"/>
+  <autoFilter ref="$A$1:$Z$999">
+    <sortState ref="A1:Z999">
+      <sortCondition ref="B1:B999"/>
     </sortState>
   </autoFilter>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Changed x axis on sample brightness graph
</commit_message>
<xml_diff>
--- a/EMPANADA Data Files Key.xlsx
+++ b/EMPANADA Data Files Key.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
   <si>
     <t>Original File Name:</t>
   </si>
@@ -259,7 +259,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -274,7 +274,13 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <name val="Serif"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Serif"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -290,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -302,6 +308,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -573,10 +582,10 @@
         <v>210.0</v>
       </c>
       <c r="F2" s="4">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="G2" s="4">
-        <v>20.0</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="3">
@@ -596,10 +605,10 @@
         <v>70.0</v>
       </c>
       <c r="F3" s="4">
-        <v>15.0</v>
+        <v>17.0</v>
       </c>
       <c r="G3" s="4">
-        <v>44.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="4">
@@ -618,10 +627,10 @@
       <c r="E4" s="2">
         <v>130.0</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <v>11.0</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="2">
         <v>27.0</v>
       </c>
     </row>
@@ -641,10 +650,10 @@
       <c r="E5" s="2">
         <v>210.0</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <v>9.0</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="2">
         <v>20.0</v>
       </c>
     </row>
@@ -664,10 +673,10 @@
       <c r="E6" s="2">
         <v>70.0</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>4.0</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="2">
         <v>32.0</v>
       </c>
     </row>
@@ -684,13 +693,13 @@
       <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <v>110.0</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="2">
         <v>9.0</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="2">
         <v>30.0</v>
       </c>
     </row>
@@ -707,13 +716,13 @@
       <c r="D8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="2">
         <v>110.0</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="2">
         <v>6.0</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="2">
         <v>30.0</v>
       </c>
     </row>
@@ -730,13 +739,13 @@
       <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="2">
         <v>130.0</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="2">
         <v>7.0</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="2">
         <v>28.0</v>
       </c>
     </row>
@@ -753,13 +762,13 @@
       <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="2">
         <v>130.0</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="2">
         <v>6.0</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="2">
         <v>27.0</v>
       </c>
     </row>
@@ -776,13 +785,13 @@
       <c r="D11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="2">
         <v>130.0</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="2">
         <v>6.0</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="2">
         <v>26.0</v>
       </c>
     </row>
@@ -799,16 +808,16 @@
       <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="2">
         <v>150.0</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="2">
         <v>8.0</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="2">
         <v>24.0</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -825,13 +834,13 @@
       <c r="D13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="2">
         <v>150.0</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="2">
         <v>7.0</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="2">
         <v>26.0</v>
       </c>
     </row>
@@ -848,13 +857,13 @@
       <c r="D14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="2">
         <v>150.0</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="2">
         <v>6.0</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="2">
         <v>24.0</v>
       </c>
     </row>
@@ -871,13 +880,13 @@
       <c r="D15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="2">
         <v>170.0</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="2">
         <v>7.0</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="2">
         <v>24.0</v>
       </c>
     </row>
@@ -894,13 +903,13 @@
       <c r="D16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="2">
         <v>170.0</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="2">
         <v>7.0</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="2">
         <v>22.0</v>
       </c>
     </row>
@@ -917,13 +926,13 @@
       <c r="D17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="2">
         <v>170.0</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="2">
         <v>6.0</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="2">
         <v>22.0</v>
       </c>
     </row>
@@ -940,13 +949,13 @@
       <c r="D18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="2">
         <v>190.0</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="2">
         <v>7.0</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="2">
         <v>21.0</v>
       </c>
     </row>
@@ -963,13 +972,13 @@
       <c r="D19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="2">
         <v>190.0</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="2">
         <v>7.0</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="2">
         <v>21.0</v>
       </c>
     </row>
@@ -986,16 +995,16 @@
       <c r="D20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="2">
         <v>210.0</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="2">
         <v>6.0</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="2">
         <v>20.0</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1012,13 +1021,13 @@
       <c r="D21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="2">
         <v>210.0</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="2">
         <v>7.0</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="2">
         <v>20.0</v>
       </c>
     </row>
@@ -1035,13 +1044,13 @@
       <c r="D22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="2">
         <v>210.0</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="2">
         <v>6.0</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="2">
         <v>20.0</v>
       </c>
     </row>
@@ -1058,13 +1067,13 @@
       <c r="D23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="2">
         <v>210.0</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="2">
         <v>7.0</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="2">
         <v>20.0</v>
       </c>
     </row>
@@ -1081,13 +1090,13 @@
       <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="2">
         <v>210.0</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="2">
         <v>6.0</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="2">
         <v>19.0</v>
       </c>
     </row>
@@ -1104,13 +1113,13 @@
       <c r="D25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="2">
         <v>230.0</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="2">
         <v>7.0</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="2">
         <v>19.0</v>
       </c>
     </row>
@@ -1127,13 +1136,13 @@
       <c r="D26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="2">
         <v>230.0</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="2">
         <v>6.0</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="2">
         <v>19.0</v>
       </c>
     </row>
@@ -1150,13 +1159,13 @@
       <c r="D27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="2">
         <v>70.0</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="2">
         <v>16.0</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="2">
         <v>42.0</v>
       </c>
     </row>
@@ -1173,16 +1182,16 @@
       <c r="D28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="2">
         <v>70.0</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="2">
         <v>7.0</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="2">
         <v>43.0</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1199,14 +1208,17 @@
       <c r="D29" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="2">
         <v>70.0</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="2">
         <v>7.0</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="2">
         <v>42.0</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="30">
@@ -1222,13 +1234,13 @@
       <c r="D30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="2">
         <v>90.0</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="2">
         <v>7.0</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="2">
         <v>35.0</v>
       </c>
     </row>
@@ -1245,16 +1257,16 @@
       <c r="D31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="2">
         <v>90.0</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="2">
         <v>7.0</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="2">
         <v>34.0</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H31" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1276,10 +1288,10 @@
         <v>210.0</v>
       </c>
       <c r="F32" s="4">
-        <v>6.0</v>
+        <v>6.5</v>
       </c>
       <c r="G32" s="4">
-        <v>19.0</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="33">
@@ -1293,17 +1305,17 @@
       <c r="C33" s="2">
         <v>2.0</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="2">
         <v>70.0</v>
       </c>
       <c r="F33" s="4">
-        <v>7.0</v>
+        <v>10.0</v>
       </c>
       <c r="G33" s="4">
-        <v>42.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="34">
@@ -1323,10 +1335,10 @@
       <c r="E34" s="2">
         <v>130.0</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="2">
         <v>7.0</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="2">
         <v>26.0</v>
       </c>
     </row>
@@ -1347,10 +1359,10 @@
       <c r="E35" s="2">
         <v>210.0</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="2">
         <v>6.0</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="2">
         <v>19.0</v>
       </c>
     </row>
@@ -1368,13 +1380,13 @@
       <c r="D36" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="2">
         <v>70.0</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="2">
         <v>0.0</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="2">
         <v>33.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added derivative comparison graph in brightness postprocessing
</commit_message>
<xml_diff>
--- a/EMPANADA Data Files Key.xlsx
+++ b/EMPANADA Data Files Key.xlsx
@@ -39,40 +39,97 @@
     <t>Questionable:</t>
   </si>
   <si>
+    <t>2018-11-13 07.33.47.mov</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>2018-11-13 07.55.37.mov</t>
+  </si>
+  <si>
+    <t>Day1-Martian-70mms.mov</t>
+  </si>
+  <si>
+    <t>Martian</t>
+  </si>
+  <si>
+    <t>2018-11-13 07.56.49.mov</t>
+  </si>
+  <si>
+    <t>Day1-Martian-210mms.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 07.58.04.mov</t>
+  </si>
+  <si>
+    <t>Day1-Martian-130mms.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 07.59.29.mov</t>
+  </si>
+  <si>
+    <t>Day1-Lunar-70mms-1.mov</t>
+  </si>
+  <si>
+    <t>Lunar</t>
+  </si>
+  <si>
     <t>2018-11-13 08.00.45.mov</t>
   </si>
   <si>
     <t>Day1-Lunar-210mms.mov</t>
   </si>
   <si>
-    <t>Lunar</t>
-  </si>
-  <si>
-    <t>2018-11-13 07.59.29.mov</t>
-  </si>
-  <si>
-    <t>Day1-Lunar-70mms.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 07.58.04.mov</t>
-  </si>
-  <si>
-    <t>Day1-Martian-130mms.mov</t>
-  </si>
-  <si>
-    <t>Martian</t>
-  </si>
-  <si>
-    <t>2018-11-13 07.56.49.mov</t>
-  </si>
-  <si>
-    <t>Day1-Martian-210mms.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 07.55.37.mov</t>
-  </si>
-  <si>
-    <t>Day1-Martian-70mms.mov</t>
+    <t>2018-11-13 08.03.53.mov</t>
+  </si>
+  <si>
+    <t>Day1-Lunar-70mms-2.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.05.13.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-210mms-1.mov</t>
+  </si>
+  <si>
+    <t>Micro</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.06.30.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-150mms-1.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.07.49.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-130mms-1.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.09.07.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-170mms-1.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.14.47.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-90mms-1.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.16.05.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-230mms-1.mov</t>
   </si>
   <si>
     <t>2018-11-13 08.17.18.mov</t>
@@ -81,7 +138,58 @@
     <t>Day1-Micro-110mms-1.mov</t>
   </si>
   <si>
-    <t>Micro</t>
+    <t>2018-11-13 08.18.38.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-190mms-1.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.19.57.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-210mms-2.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.23.12.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-70mms-2.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.24.30.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-210mms-3.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.25.45.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-150mms-2.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.27.10.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-130mms-2.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.28.29.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-170mms-2.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.32.20.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-90mms-2.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.33.38.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-230mms-2.mov</t>
   </si>
   <si>
     <t>2018-11-13 08.34.56.mov</t>
@@ -90,16 +198,34 @@
     <t>Day1-Micro-110mms-2.mov</t>
   </si>
   <si>
-    <t>2018-11-13 08.07.49.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-130mms-1.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.27.10.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-130mms-2.mov</t>
+    <t>2018-11-13 08.36.14.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-190mms-2.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.37.34.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-210mms-4.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.40.00.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-70mms-3.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.41.17.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-210mms-5.mov</t>
+  </si>
+  <si>
+    <t>2018-11-13 08.42.37.mov</t>
+  </si>
+  <si>
+    <t>Day1-Micro-150mms-3.mov</t>
   </si>
   <si>
     <t>2018-11-13 08.43.55.mov</t>
@@ -108,158 +234,32 @@
     <t>Day1-Micro-130mms-3.mov</t>
   </si>
   <si>
-    <t>2018-11-13 08.06.30.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-150mms-1.mov</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.25.45.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-150mms-2.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.42.37.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-150mms-3.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.09.07.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-170mms-1.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.28.29.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-170mms-2.mov</t>
-  </si>
-  <si>
     <t>2018-11-13 08.45.13.mov</t>
   </si>
   <si>
     <t>Day1-Micro-170mms-3.mov</t>
   </si>
   <si>
-    <t>2018-11-13 08.18.38.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-190mms-1.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.36.14.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-190mms-2.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.05.13.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-210mms-1.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.19.57.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-210mms-2.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.24.30.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-210mms-3.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.37.34.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-210mms-4.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.41.17.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-210mms-5.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.16.05.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-230mms-1.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.33.38.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-230mms-2.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.03.53.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-70mms-1.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.23.12.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-70mms-2.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.40.00.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-70mms-3.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.14.47.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-90mms-1.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 08.32.20.mov</t>
-  </si>
-  <si>
-    <t>Day1-Micro-90mms-2.mov</t>
+    <t>2018-11-14 08.42.19.mov</t>
+  </si>
+  <si>
+    <t>2018-11-14 08.43.36.mov</t>
+  </si>
+  <si>
+    <t>2018-11-14 08.44.42.mov</t>
+  </si>
+  <si>
+    <t>2018-11-14 08.48.47.mov</t>
   </si>
   <si>
     <t>2018-11-14 08.49.53.mov</t>
-  </si>
-  <si>
-    <t>2018-11-14 08.48.47.mov</t>
-  </si>
-  <si>
-    <t>2018-11-14 08.44.42.mov</t>
-  </si>
-  <si>
-    <t>2018-11-14 08.43.36.mov</t>
-  </si>
-  <si>
-    <t>2018-11-14 08.42.19.mov</t>
-  </si>
-  <si>
-    <t>2018-11-13 07.33.47.mov</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Earth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -274,6 +274,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <name val="Serif"/>
     </font>
@@ -296,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -311,6 +312,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -569,7 +573,7 @@
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="2">
@@ -577,15 +581,6 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="2">
-        <v>210.0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>9.0</v>
-      </c>
-      <c r="G2" s="4">
-        <v>18.5</v>
       </c>
     </row>
     <row r="3">
@@ -599,39 +594,39 @@
         <v>1.0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
         <v>70.0</v>
       </c>
-      <c r="F3" s="4">
-        <v>17.0</v>
-      </c>
-      <c r="G3" s="4">
-        <v>42.0</v>
+      <c r="F3" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>32.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" s="2">
-        <v>130.0</v>
+        <v>210.0</v>
       </c>
       <c r="F4" s="2">
-        <v>11.0</v>
+        <v>9.0</v>
       </c>
       <c r="G4" s="2">
-        <v>27.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="5">
@@ -645,85 +640,85 @@
         <v>1.0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2">
-        <v>210.0</v>
+        <v>130.0</v>
       </c>
       <c r="F5" s="2">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="G5" s="2">
-        <v>20.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="2">
         <v>1.0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2">
         <v>70.0</v>
       </c>
-      <c r="F6" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>32.0</v>
+      <c r="F6" s="5">
+        <v>17.0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>42.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E7" s="2">
-        <v>110.0</v>
-      </c>
-      <c r="F7" s="2">
+        <v>210.0</v>
+      </c>
+      <c r="F7" s="5">
         <v>9.0</v>
       </c>
-      <c r="G7" s="2">
-        <v>30.0</v>
+      <c r="G7" s="5">
+        <v>18.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="2">
         <v>1.0</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
+      <c r="D8" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="E8" s="2">
-        <v>110.0</v>
+        <v>70.0</v>
       </c>
       <c r="F8" s="2">
-        <v>6.0</v>
+        <v>16.0</v>
       </c>
       <c r="G8" s="2">
-        <v>30.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="9">
@@ -737,361 +732,367 @@
         <v>1.0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2">
-        <v>130.0</v>
+        <v>210.0</v>
       </c>
       <c r="F9" s="2">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="G9" s="2">
-        <v>28.0</v>
+        <v>20.0</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="2">
+        <v>150.0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>24.0</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="2">
-        <v>130.0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="G10" s="2">
-        <v>27.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2">
         <v>1.0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E11" s="2">
         <v>130.0</v>
       </c>
       <c r="F11" s="2">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="G11" s="2">
-        <v>26.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2">
         <v>1.0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E12" s="2">
-        <v>150.0</v>
+        <v>170.0</v>
       </c>
       <c r="F12" s="2">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="G12" s="2">
         <v>24.0</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" s="2">
         <v>1.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E13" s="2">
-        <v>150.0</v>
+        <v>90.0</v>
       </c>
       <c r="F13" s="2">
         <v>7.0</v>
       </c>
       <c r="G13" s="2">
-        <v>26.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2">
         <v>1.0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E14" s="2">
-        <v>150.0</v>
+        <v>230.0</v>
       </c>
       <c r="F14" s="2">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="G14" s="2">
-        <v>24.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" s="2">
         <v>1.0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E15" s="2">
-        <v>170.0</v>
+        <v>110.0</v>
       </c>
       <c r="F15" s="2">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="G15" s="2">
-        <v>24.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C16" s="2">
         <v>1.0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E16" s="2">
-        <v>170.0</v>
+        <v>190.0</v>
       </c>
       <c r="F16" s="2">
         <v>7.0</v>
       </c>
       <c r="G16" s="2">
-        <v>22.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C17" s="2">
         <v>1.0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E17" s="2">
-        <v>170.0</v>
+        <v>210.0</v>
       </c>
       <c r="F17" s="2">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="G17" s="2">
-        <v>22.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" s="2">
         <v>1.0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E18" s="2">
-        <v>190.0</v>
+        <v>70.0</v>
       </c>
       <c r="F18" s="2">
         <v>7.0</v>
       </c>
       <c r="G18" s="2">
-        <v>21.0</v>
+        <v>43.0</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" s="2">
         <v>1.0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E19" s="2">
-        <v>190.0</v>
+        <v>210.0</v>
       </c>
       <c r="F19" s="2">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="G19" s="2">
-        <v>21.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" s="2">
         <v>1.0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E20" s="2">
-        <v>210.0</v>
+        <v>150.0</v>
       </c>
       <c r="F20" s="2">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="G20" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>33</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C21" s="2">
         <v>1.0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E21" s="2">
-        <v>210.0</v>
+        <v>130.0</v>
       </c>
       <c r="F21" s="2">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="G21" s="2">
-        <v>20.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" s="2">
         <v>1.0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E22" s="2">
-        <v>210.0</v>
+        <v>170.0</v>
       </c>
       <c r="F22" s="2">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="G22" s="2">
-        <v>20.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" s="2">
         <v>1.0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E23" s="2">
-        <v>210.0</v>
+        <v>90.0</v>
       </c>
       <c r="F23" s="2">
         <v>7.0</v>
       </c>
       <c r="G23" s="2">
-        <v>20.0</v>
+        <v>34.0</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C24" s="2">
         <v>1.0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E24" s="2">
-        <v>210.0</v>
+        <v>230.0</v>
       </c>
       <c r="F24" s="2">
         <v>6.0</v>
@@ -1102,85 +1103,85 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C25" s="2">
         <v>1.0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E25" s="2">
-        <v>230.0</v>
+        <v>110.0</v>
       </c>
       <c r="F25" s="2">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="G25" s="2">
-        <v>19.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C26" s="2">
         <v>1.0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E26" s="2">
-        <v>230.0</v>
+        <v>190.0</v>
       </c>
       <c r="F26" s="2">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="G26" s="2">
-        <v>19.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C27" s="2">
         <v>1.0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E27" s="2">
-        <v>70.0</v>
+        <v>210.0</v>
       </c>
       <c r="F27" s="2">
-        <v>16.0</v>
+        <v>7.0</v>
       </c>
       <c r="G27" s="2">
-        <v>42.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C28" s="2">
         <v>1.0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E28" s="2">
         <v>70.0</v>
@@ -1189,224 +1190,228 @@
         <v>7.0</v>
       </c>
       <c r="G28" s="2">
-        <v>43.0</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>33</v>
+        <v>42.0</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C29" s="2">
         <v>1.0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E29" s="2">
-        <v>70.0</v>
+        <v>210.0</v>
       </c>
       <c r="F29" s="2">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="G29" s="2">
-        <v>42.0</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>33</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C30" s="2">
         <v>1.0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E30" s="2">
-        <v>90.0</v>
+        <v>150.0</v>
       </c>
       <c r="F30" s="2">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="G30" s="2">
-        <v>35.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C31" s="2">
         <v>1.0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E31" s="2">
-        <v>90.0</v>
+        <v>130.0</v>
       </c>
       <c r="F31" s="2">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="G31" s="2">
-        <v>34.0</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>33</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="3" t="str">
-        <f t="shared" ref="B32:B36" si="1">"Day"&amp;C32&amp;"-"&amp;D32&amp;"-"&amp;E32&amp;"mms.mov"</f>
-        <v>Day2-Lunar-210mms.mov</v>
+        <v>73</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="C32" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E32" s="2">
-        <v>210.0</v>
-      </c>
-      <c r="F32" s="4">
-        <v>6.5</v>
-      </c>
-      <c r="G32" s="4">
-        <v>18.5</v>
+        <v>170.0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="G32" s="2">
+        <v>22.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B33" s="3" t="str">
+        <f t="shared" ref="B33:B37" si="1">"Day"&amp;C33&amp;"-"&amp;D33&amp;"-"&amp;E33&amp;"mms.mov"</f>
+        <v>Day2-Martian-70mms.mov</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="2">
+        <v>70.0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G33" s="2">
+        <v>33.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Day2-Martian-210mms.mov</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="2">
+        <v>210.0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="G34" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Day2-Martian-130mms.mov</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="2">
+        <v>130.0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="G35" s="2">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Day2-Lunar-70mms.mov</v>
       </c>
-      <c r="C33" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="2">
-        <v>70.0</v>
-      </c>
-      <c r="F33" s="4">
-        <v>10.0</v>
-      </c>
-      <c r="G33" s="4">
-        <v>41.0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B34" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Day2-Martian-130mms.mov</v>
-      </c>
-      <c r="C34" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="2">
-        <v>130.0</v>
-      </c>
-      <c r="F34" s="2">
-        <v>7.0</v>
-      </c>
-      <c r="G34" s="2">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B35" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Day2-Martian-210mms.mov</v>
-      </c>
-      <c r="C35" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="2">
-        <v>210.0</v>
-      </c>
-      <c r="F35" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="G35" s="2">
-        <v>19.0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B36" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>Day2-Martian-70mms.mov</v>
-      </c>
       <c r="C36" s="2">
         <v>2.0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E36" s="2">
         <v>70.0</v>
       </c>
-      <c r="F36" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="G36" s="2">
-        <v>33.0</v>
+      <c r="F36" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="G36" s="5">
+        <v>41.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="B37" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Day2-Lunar-210mms.mov</v>
       </c>
       <c r="C37" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>79</v>
+        <v>20</v>
+      </c>
+      <c r="E37" s="2">
+        <v>210.0</v>
+      </c>
+      <c r="F37" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="G37" s="5">
+        <v>18.5</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="$A$1:$Z$999">
     <sortState ref="A1:Z999">
+      <sortCondition ref="A1:A999"/>
       <sortCondition ref="B1:B999"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Added new Earth data!
</commit_message>
<xml_diff>
--- a/EMPANADA Data Files Key.xlsx
+++ b/EMPANADA Data Files Key.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="81">
   <si>
     <t>Original File Name:</t>
   </si>
@@ -253,13 +253,16 @@
   </si>
   <si>
     <t>2018-11-14 08.49.53.mov</t>
+  </si>
+  <si>
+    <t>Day3-Earth-130mms.mov</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -273,10 +276,6 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
-      <name val="Serif"/>
     </font>
     <font>
       <color theme="1"/>
@@ -297,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -309,12 +308,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -656,7 +649,7 @@
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="2">
@@ -668,10 +661,10 @@
       <c r="E6" s="2">
         <v>70.0</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>17.0</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>42.0</v>
       </c>
     </row>
@@ -691,10 +684,10 @@
       <c r="E7" s="2">
         <v>210.0</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>9.0</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>18.5</v>
       </c>
     </row>
@@ -702,13 +695,13 @@
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="2">
         <v>1.0</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="2">
@@ -1192,7 +1185,7 @@
       <c r="G28" s="2">
         <v>42.0</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H28" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1377,10 +1370,10 @@
       <c r="E36" s="2">
         <v>70.0</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F36" s="4">
         <v>10.0</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="4">
         <v>41.0</v>
       </c>
     </row>
@@ -1401,11 +1394,34 @@
       <c r="E37" s="2">
         <v>210.0</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F37" s="4">
         <v>6.5</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="4">
         <v>18.5</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="2">
+        <v>130.0</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G38" s="2">
+        <v>7.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Day 3 and 4 data, and added support for Earth gravity
</commit_message>
<xml_diff>
--- a/EMPANADA Data Files Key.xlsx
+++ b/EMPANADA Data Files Key.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="122">
   <si>
     <t>Original File Name:</t>
   </si>
@@ -57,12 +57,18 @@
     <t>Martian</t>
   </si>
   <si>
+    <t>A note about speeds:</t>
+  </si>
+  <si>
     <t>2018-11-13 07.56.49.mov</t>
   </si>
   <si>
     <t>Day1-Martian-210mms.mov</t>
   </si>
   <si>
+    <t>It turns out that the old speeds (days 1 and 2) are all wrong, but instead of changing the names, I have just accounted for this in the program. The reason I don't want to change the names is because all of the new speeds are decimals, but they ranges for ~2.5mm/s to ~8.5mm/s. See LABlog for more info, specifically June 1-2, 2020</t>
+  </si>
+  <si>
     <t>2018-11-13 07.58.04.mov</t>
   </si>
   <si>
@@ -255,14 +261,131 @@
     <t>2018-11-14 08.49.53.mov</t>
   </si>
   <si>
-    <t>Day3-Earth-130mms.mov</t>
+    <t>IMG_1110.MOV</t>
+  </si>
+  <si>
+    <t>Day3-Earth-1mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1111.MOV</t>
+  </si>
+  <si>
+    <t>Day3-Earth-2mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1112.MOV</t>
+  </si>
+  <si>
+    <t>Day3-Earth-3mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1113.MOV</t>
+  </si>
+  <si>
+    <t>Day3-Earth-4mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1115.MOV</t>
+  </si>
+  <si>
+    <t>Day3-Earth-5mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1116.MOV</t>
+  </si>
+  <si>
+    <t>Day3-Earth-6mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1117.MOV</t>
+  </si>
+  <si>
+    <t>Day3-Earth-7mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1118.MOV</t>
+  </si>
+  <si>
+    <t>Day3-Earth-8mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1119.MOV</t>
+  </si>
+  <si>
+    <t>Day3-Earth-9mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1120.MOV</t>
+  </si>
+  <si>
+    <t>Day3-Earth-10mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1134.MOV</t>
+  </si>
+  <si>
+    <t>Day4-Earth-1mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1135.MOV</t>
+  </si>
+  <si>
+    <t>Day4-Earth-2mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1136.MOV</t>
+  </si>
+  <si>
+    <t>Day4-Earth-3mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1137.MOV</t>
+  </si>
+  <si>
+    <t>Day4-Earth-4mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1138.MOV</t>
+  </si>
+  <si>
+    <t>Day4-Earth-5mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1139.MOV</t>
+  </si>
+  <si>
+    <t>Day4-Earth-6mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1140.MOV</t>
+  </si>
+  <si>
+    <t>Day4-Earth-7mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1141.MOV</t>
+  </si>
+  <si>
+    <t>Day4-Earth-8mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1142.MOV</t>
+  </si>
+  <si>
+    <t>Day4-Earth-9mms.mov</t>
+  </si>
+  <si>
+    <t>IMG_1143.MOV</t>
+  </si>
+  <si>
+    <t>Day4-Earth-10mms.mov</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -281,6 +404,7 @@
       <color theme="1"/>
       <name val="Serif"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -296,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -308,6 +432,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -534,6 +661,7 @@
     <col customWidth="1" min="6" max="6" width="18.86"/>
     <col customWidth="1" min="7" max="7" width="17.14"/>
     <col customWidth="1" min="8" max="8" width="16.29"/>
+    <col customWidth="1" min="10" max="10" width="20.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -598,13 +726,16 @@
       <c r="G3" s="2">
         <v>32.0</v>
       </c>
+      <c r="J3" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2">
         <v>1.0</v>
@@ -621,13 +752,16 @@
       <c r="G4" s="2">
         <v>20.0</v>
       </c>
+      <c r="J4" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2">
         <v>1.0</v>
@@ -647,16 +781,16 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2">
         <v>1.0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2">
         <v>70.0</v>
@@ -670,16 +804,16 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E7" s="2">
         <v>210.0</v>
@@ -693,16 +827,16 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2">
         <v>1.0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E8" s="2">
         <v>70.0</v>
@@ -716,16 +850,16 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2">
         <v>1.0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E9" s="2">
         <v>210.0</v>
@@ -737,21 +871,21 @@
         <v>20.0</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2">
         <v>1.0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2">
         <v>150.0</v>
@@ -763,21 +897,21 @@
         <v>24.0</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" s="2">
         <v>1.0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2">
         <v>130.0</v>
@@ -791,16 +925,16 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C12" s="2">
         <v>1.0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E12" s="2">
         <v>170.0</v>
@@ -814,16 +948,16 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13" s="2">
         <v>1.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E13" s="2">
         <v>90.0</v>
@@ -837,16 +971,16 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2">
         <v>1.0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E14" s="2">
         <v>230.0</v>
@@ -860,16 +994,16 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C15" s="2">
         <v>1.0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E15" s="2">
         <v>110.0</v>
@@ -883,16 +1017,16 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C16" s="2">
         <v>1.0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E16" s="2">
         <v>190.0</v>
@@ -906,16 +1040,16 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C17" s="2">
         <v>1.0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E17" s="2">
         <v>210.0</v>
@@ -929,16 +1063,16 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C18" s="2">
         <v>1.0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E18" s="2">
         <v>70.0</v>
@@ -950,21 +1084,21 @@
         <v>43.0</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C19" s="2">
         <v>1.0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E19" s="2">
         <v>210.0</v>
@@ -978,16 +1112,16 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C20" s="2">
         <v>1.0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E20" s="2">
         <v>150.0</v>
@@ -1001,16 +1135,16 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C21" s="2">
         <v>1.0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E21" s="2">
         <v>130.0</v>
@@ -1024,16 +1158,16 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2">
         <v>1.0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E22" s="2">
         <v>170.0</v>
@@ -1047,16 +1181,16 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C23" s="2">
         <v>1.0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E23" s="2">
         <v>90.0</v>
@@ -1068,21 +1202,21 @@
         <v>34.0</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C24" s="2">
         <v>1.0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E24" s="2">
         <v>230.0</v>
@@ -1096,16 +1230,16 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C25" s="2">
         <v>1.0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E25" s="2">
         <v>110.0</v>
@@ -1119,16 +1253,16 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C26" s="2">
         <v>1.0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E26" s="2">
         <v>190.0</v>
@@ -1142,16 +1276,16 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C27" s="2">
         <v>1.0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E27" s="2">
         <v>210.0</v>
@@ -1165,16 +1299,16 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C28" s="2">
         <v>1.0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E28" s="2">
         <v>70.0</v>
@@ -1186,21 +1320,21 @@
         <v>42.0</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C29" s="2">
         <v>1.0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E29" s="2">
         <v>210.0</v>
@@ -1214,16 +1348,16 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C30" s="2">
         <v>1.0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E30" s="2">
         <v>150.0</v>
@@ -1237,16 +1371,16 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C31" s="2">
         <v>1.0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E31" s="2">
         <v>130.0</v>
@@ -1260,16 +1394,16 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C32" s="2">
         <v>1.0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E32" s="2">
         <v>170.0</v>
@@ -1283,7 +1417,7 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B33" s="3" t="str">
         <f t="shared" ref="B33:B37" si="1">"Day"&amp;C33&amp;"-"&amp;D33&amp;"-"&amp;E33&amp;"mms.mov"</f>
@@ -1307,7 +1441,7 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B34" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1331,7 +1465,7 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B35" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1355,7 +1489,7 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B36" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1365,7 +1499,7 @@
         <v>2.0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E36" s="2">
         <v>70.0</v>
@@ -1379,7 +1513,7 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B37" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1389,7 +1523,7 @@
         <v>2.0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E37" s="2">
         <v>210.0</v>
@@ -1402,11 +1536,11 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>80</v>
+      <c r="A38" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="C38" s="2">
         <v>3.0</v>
@@ -1414,14 +1548,451 @@
       <c r="D38" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="2">
-        <v>130.0</v>
+      <c r="E38" s="5">
+        <v>1.0</v>
       </c>
       <c r="F38" s="2">
-        <v>0.0</v>
+        <v>72.0</v>
       </c>
       <c r="G38" s="2">
+        <v>120.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="F39" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="G39" s="2">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="F40" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="G40" s="2">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="F41" s="2">
         <v>7.0</v>
+      </c>
+      <c r="G41" s="2">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="F42" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="G42" s="2">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="F43" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="G43" s="2">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="F44" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="G44" s="2">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="F45" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="G45" s="2">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="F46" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="G46" s="2">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="F47" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G47" s="2">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F48" s="2">
+        <v>30.0</v>
+      </c>
+      <c r="G48" s="2">
+        <v>122.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F49" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="G49" s="2">
+        <v>56.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="F50" s="2">
+        <v>13.0</v>
+      </c>
+      <c r="G50" s="2">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="F51" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="G51" s="2">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="F52" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="G52" s="2">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="F53" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="G53" s="2">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="F54" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="G54" s="2">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="F55" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G55" s="2">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="F56" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G56" s="2">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="F57" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G57" s="2">
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created figures with day 5 tests
</commit_message>
<xml_diff>
--- a/EMPANADA Data Files Key.xlsx
+++ b/EMPANADA Data Files Key.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="124">
   <si>
     <t>Original File Name:</t>
   </si>
@@ -379,6 +379,12 @@
   </si>
   <si>
     <t>Day4-Earth-10mms.mov</t>
+  </si>
+  <si>
+    <t>Day5-Earth-8mms.mov</t>
+  </si>
+  <si>
+    <t>Day5-Earth-2mms.mov</t>
   </si>
 </sst>
 </file>
@@ -1536,10 +1542,10 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C38" s="2">
@@ -1548,7 +1554,7 @@
       <c r="D38" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="2">
         <v>1.0</v>
       </c>
       <c r="F38" s="2">
@@ -1559,10 +1565,10 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="2">
@@ -1571,7 +1577,7 @@
       <c r="D39" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="2">
         <v>2.0</v>
       </c>
       <c r="F39" s="2">
@@ -1582,7 +1588,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1594,7 +1600,7 @@
       <c r="D40" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="2">
         <v>3.0</v>
       </c>
       <c r="F40" s="2">
@@ -1608,7 +1614,7 @@
       <c r="A41" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C41" s="2">
@@ -1617,7 +1623,7 @@
       <c r="D41" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41" s="2">
         <v>4.0</v>
       </c>
       <c r="F41" s="2">
@@ -1631,7 +1637,7 @@
       <c r="A42" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C42" s="2">
@@ -1640,7 +1646,7 @@
       <c r="D42" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="2">
         <v>5.0</v>
       </c>
       <c r="F42" s="2">
@@ -1654,7 +1660,7 @@
       <c r="A43" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C43" s="2">
@@ -1663,7 +1669,7 @@
       <c r="D43" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="2">
         <v>6.0</v>
       </c>
       <c r="F43" s="2">
@@ -1677,7 +1683,7 @@
       <c r="A44" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C44" s="2">
@@ -1686,7 +1692,7 @@
       <c r="D44" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="2">
         <v>7.0</v>
       </c>
       <c r="F44" s="2">
@@ -1700,7 +1706,7 @@
       <c r="A45" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C45" s="2">
@@ -1709,7 +1715,7 @@
       <c r="D45" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E45" s="2">
         <v>8.0</v>
       </c>
       <c r="F45" s="2">
@@ -1723,7 +1729,7 @@
       <c r="A46" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C46" s="2">
@@ -1732,7 +1738,7 @@
       <c r="D46" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46" s="2">
         <v>9.0</v>
       </c>
       <c r="F46" s="2">
@@ -1746,7 +1752,7 @@
       <c r="A47" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="2" t="s">
         <v>101</v>
       </c>
       <c r="C47" s="2">
@@ -1755,7 +1761,7 @@
       <c r="D47" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="2">
         <v>10.0</v>
       </c>
       <c r="F47" s="2">
@@ -1766,10 +1772,10 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="2" t="s">
         <v>103</v>
       </c>
       <c r="C48" s="2">
@@ -1789,10 +1795,10 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C49" s="2">
@@ -1812,10 +1818,10 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="2" t="s">
         <v>107</v>
       </c>
       <c r="C50" s="2">
@@ -1835,10 +1841,10 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="2" t="s">
         <v>109</v>
       </c>
       <c r="C51" s="2">
@@ -1858,10 +1864,10 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C52" s="2">
@@ -1881,10 +1887,10 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C53" s="2">
@@ -1904,10 +1910,10 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="2" t="s">
         <v>115</v>
       </c>
       <c r="C54" s="2">
@@ -1927,10 +1933,10 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C55" s="2">
@@ -1950,10 +1956,10 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C56" s="2">
@@ -1973,10 +1979,10 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C57" s="2">
@@ -1993,6 +1999,52 @@
       </c>
       <c r="G57" s="2">
         <v>10.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="F58" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G58" s="2">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F59" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="G59" s="2">
+        <v>50.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleted days 3 and 4 because they were bad, retook day 3, much better results
</commit_message>
<xml_diff>
--- a/EMPANADA Data Files Key.xlsx
+++ b/EMPANADA Data Files Key.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="114">
   <si>
     <t>Original File Name:</t>
   </si>
@@ -261,121 +261,91 @@
     <t>2018-11-14 08.49.53.mov</t>
   </si>
   <si>
-    <t>IMG_1110.MOV</t>
+    <t>MVI_0619.MOV</t>
   </si>
   <si>
     <t>Day3-Earth-1mms.mov</t>
   </si>
   <si>
-    <t>IMG_1111.MOV</t>
+    <t>MVI_0620.MOV</t>
   </si>
   <si>
     <t>Day3-Earth-2mms.mov</t>
   </si>
   <si>
-    <t>IMG_1112.MOV</t>
+    <t>MVI_0621.MOV</t>
   </si>
   <si>
     <t>Day3-Earth-3mms.mov</t>
   </si>
   <si>
-    <t>IMG_1113.MOV</t>
+    <t>MVI_0622.MOV</t>
   </si>
   <si>
     <t>Day3-Earth-4mms.mov</t>
   </si>
   <si>
-    <t>IMG_1115.MOV</t>
+    <t>MVI_0623.MOV</t>
   </si>
   <si>
     <t>Day3-Earth-5mms.mov</t>
   </si>
   <si>
-    <t>IMG_1116.MOV</t>
+    <t>MVI_0624.MOV</t>
   </si>
   <si>
     <t>Day3-Earth-6mms.mov</t>
   </si>
   <si>
-    <t>IMG_1117.MOV</t>
+    <t>MVI_0625.MOV</t>
   </si>
   <si>
     <t>Day3-Earth-7mms.mov</t>
   </si>
   <si>
-    <t>IMG_1118.MOV</t>
+    <t>MVI_0626.MOV</t>
   </si>
   <si>
     <t>Day3-Earth-8mms.mov</t>
   </si>
   <si>
-    <t>IMG_1119.MOV</t>
+    <t>MVI_0627.MOV</t>
   </si>
   <si>
     <t>Day3-Earth-9mms.mov</t>
   </si>
   <si>
-    <t>IMG_1120.MOV</t>
+    <t>MVI_0628.MOV</t>
   </si>
   <si>
     <t>Day3-Earth-10mms.mov</t>
   </si>
   <si>
-    <t>IMG_1134.MOV</t>
-  </si>
-  <si>
     <t>Day4-Earth-1mms.mov</t>
   </si>
   <si>
-    <t>IMG_1135.MOV</t>
-  </si>
-  <si>
     <t>Day4-Earth-2mms.mov</t>
   </si>
   <si>
-    <t>IMG_1136.MOV</t>
-  </si>
-  <si>
     <t>Day4-Earth-3mms.mov</t>
   </si>
   <si>
-    <t>IMG_1137.MOV</t>
-  </si>
-  <si>
     <t>Day4-Earth-4mms.mov</t>
   </si>
   <si>
-    <t>IMG_1138.MOV</t>
-  </si>
-  <si>
     <t>Day4-Earth-5mms.mov</t>
   </si>
   <si>
-    <t>IMG_1139.MOV</t>
-  </si>
-  <si>
     <t>Day4-Earth-6mms.mov</t>
   </si>
   <si>
-    <t>IMG_1140.MOV</t>
-  </si>
-  <si>
     <t>Day4-Earth-7mms.mov</t>
   </si>
   <si>
-    <t>IMG_1141.MOV</t>
-  </si>
-  <si>
     <t>Day4-Earth-8mms.mov</t>
   </si>
   <si>
-    <t>IMG_1142.MOV</t>
-  </si>
-  <si>
     <t>Day4-Earth-9mms.mov</t>
-  </si>
-  <si>
-    <t>IMG_1143.MOV</t>
   </si>
   <si>
     <t>Day4-Earth-10mms.mov</t>
@@ -1558,14 +1528,14 @@
         <v>1.0</v>
       </c>
       <c r="F38" s="2">
-        <v>72.0</v>
+        <v>2.0</v>
       </c>
       <c r="G38" s="2">
-        <v>120.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="5" t="s">
         <v>84</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1581,10 +1551,10 @@
         <v>2.0</v>
       </c>
       <c r="F39" s="2">
-        <v>17.0</v>
+        <v>4.0</v>
       </c>
       <c r="G39" s="2">
-        <v>55.0</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="40">
@@ -1604,10 +1574,10 @@
         <v>3.0</v>
       </c>
       <c r="F40" s="2">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="G40" s="2">
-        <v>35.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="41">
@@ -1627,10 +1597,10 @@
         <v>4.0</v>
       </c>
       <c r="F41" s="2">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="G41" s="2">
-        <v>27.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="42">
@@ -1650,10 +1620,10 @@
         <v>5.0</v>
       </c>
       <c r="F42" s="2">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
       <c r="G42" s="2">
-        <v>22.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="43">
@@ -1673,7 +1643,7 @@
         <v>6.0</v>
       </c>
       <c r="F43" s="2">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
       <c r="G43" s="2">
         <v>17.0</v>
@@ -1696,7 +1666,7 @@
         <v>7.0</v>
       </c>
       <c r="F44" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="G44" s="2">
         <v>15.0</v>
@@ -1719,10 +1689,10 @@
         <v>8.0</v>
       </c>
       <c r="F45" s="2">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="G45" s="2">
-        <v>13.0</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="46">
@@ -1742,10 +1712,10 @@
         <v>9.0</v>
       </c>
       <c r="F46" s="2">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="G46" s="2">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="47">
@@ -1765,18 +1735,15 @@
         <v>10.0</v>
       </c>
       <c r="F47" s="2">
-        <v>2.0</v>
+        <v>0.5</v>
       </c>
       <c r="G47" s="2">
         <v>10.0</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="C48" s="2">
         <v>4.0</v>
@@ -1787,19 +1754,10 @@
       <c r="E48" s="2">
         <v>1.0</v>
       </c>
-      <c r="F48" s="2">
-        <v>30.0</v>
-      </c>
-      <c r="G48" s="2">
-        <v>122.0</v>
-      </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="B49" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C49" s="2">
         <v>4.0</v>
@@ -1810,19 +1768,10 @@
       <c r="E49" s="2">
         <v>2.0</v>
       </c>
-      <c r="F49" s="2">
-        <v>11.0</v>
-      </c>
-      <c r="G49" s="2">
-        <v>56.0</v>
-      </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="B50" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C50" s="2">
         <v>4.0</v>
@@ -1833,19 +1782,10 @@
       <c r="E50" s="2">
         <v>3.0</v>
       </c>
-      <c r="F50" s="2">
-        <v>13.0</v>
-      </c>
-      <c r="G50" s="2">
-        <v>36.0</v>
-      </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="B51" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C51" s="2">
         <v>4.0</v>
@@ -1856,19 +1796,10 @@
       <c r="E51" s="2">
         <v>4.0</v>
       </c>
-      <c r="F51" s="2">
-        <v>9.0</v>
-      </c>
-      <c r="G51" s="2">
-        <v>27.0</v>
-      </c>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="B52" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C52" s="2">
         <v>4.0</v>
@@ -1879,19 +1810,10 @@
       <c r="E52" s="2">
         <v>5.0</v>
       </c>
-      <c r="F52" s="2">
-        <v>8.0</v>
-      </c>
-      <c r="G52" s="2">
-        <v>21.0</v>
-      </c>
     </row>
     <row r="53">
-      <c r="A53" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="B53" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C53" s="2">
         <v>4.0</v>
@@ -1902,19 +1824,10 @@
       <c r="E53" s="2">
         <v>6.0</v>
       </c>
-      <c r="F53" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="G53" s="2">
-        <v>17.0</v>
-      </c>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="B54" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C54" s="2">
         <v>4.0</v>
@@ -1925,19 +1838,10 @@
       <c r="E54" s="2">
         <v>7.0</v>
       </c>
-      <c r="F54" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="G54" s="2">
-        <v>15.0</v>
-      </c>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="B55" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C55" s="2">
         <v>4.0</v>
@@ -1948,19 +1852,10 @@
       <c r="E55" s="2">
         <v>8.0</v>
       </c>
-      <c r="F55" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="G55" s="2">
-        <v>13.0</v>
-      </c>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="B56" s="2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C56" s="2">
         <v>4.0</v>
@@ -1971,19 +1866,10 @@
       <c r="E56" s="2">
         <v>9.0</v>
       </c>
-      <c r="F56" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G56" s="2">
-        <v>12.0</v>
-      </c>
     </row>
     <row r="57">
-      <c r="A57" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="B57" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C57" s="2">
         <v>4.0</v>
@@ -1992,12 +1878,6 @@
         <v>10</v>
       </c>
       <c r="E57" s="2">
-        <v>10.0</v>
-      </c>
-      <c r="F57" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="G57" s="2">
         <v>10.0</v>
       </c>
     </row>
@@ -2006,7 +1886,7 @@
         <v>9</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C58" s="2">
         <v>5.0</v>
@@ -2029,7 +1909,7 @@
         <v>9</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C59" s="2">
         <v>5.0</v>

</xml_diff>

<commit_message>
Added day 4 data, regenerated images; slip counting looks very good
</commit_message>
<xml_diff>
--- a/EMPANADA Data Files Key.xlsx
+++ b/EMPANADA Data Files Key.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="124">
   <si>
     <t>Original File Name:</t>
   </si>
@@ -321,31 +321,61 @@
     <t>Day3-Earth-10mms.mov</t>
   </si>
   <si>
+    <t>MVI_0629.MOV</t>
+  </si>
+  <si>
     <t>Day4-Earth-1mms.mov</t>
   </si>
   <si>
+    <t>MVI_0630.MOV</t>
+  </si>
+  <si>
     <t>Day4-Earth-2mms.mov</t>
   </si>
   <si>
+    <t>MVI_0631.MOV</t>
+  </si>
+  <si>
     <t>Day4-Earth-3mms.mov</t>
   </si>
   <si>
+    <t>MVI_0632.MOV</t>
+  </si>
+  <si>
     <t>Day4-Earth-4mms.mov</t>
   </si>
   <si>
+    <t>MVI_0633.MOV</t>
+  </si>
+  <si>
     <t>Day4-Earth-5mms.mov</t>
   </si>
   <si>
+    <t>MVI_0634.MOV</t>
+  </si>
+  <si>
     <t>Day4-Earth-6mms.mov</t>
   </si>
   <si>
+    <t>MVI_0635.MOV</t>
+  </si>
+  <si>
     <t>Day4-Earth-7mms.mov</t>
   </si>
   <si>
+    <t>MVI_0636.MOV</t>
+  </si>
+  <si>
     <t>Day4-Earth-8mms.mov</t>
   </si>
   <si>
+    <t>MVI_0637.MOV</t>
+  </si>
+  <si>
     <t>Day4-Earth-9mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0638.MOV</t>
   </si>
   <si>
     <t>Day4-Earth-10mms.mov</t>
@@ -1533,6 +1563,9 @@
       <c r="G38" s="2">
         <v>38.0</v>
       </c>
+      <c r="H38" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
@@ -1742,8 +1775,11 @@
       </c>
     </row>
     <row r="48">
+      <c r="A48" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="B48" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C48" s="2">
         <v>4.0</v>
@@ -1754,10 +1790,22 @@
       <c r="E48" s="2">
         <v>1.0</v>
       </c>
+      <c r="F48" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="G48" s="2">
+        <v>117.0</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="49">
+      <c r="A49" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="B49" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C49" s="2">
         <v>4.0</v>
@@ -1768,10 +1816,19 @@
       <c r="E49" s="2">
         <v>2.0</v>
       </c>
+      <c r="F49" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="G49" s="2">
+        <v>52.0</v>
+      </c>
     </row>
     <row r="50">
+      <c r="A50" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="B50" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C50" s="2">
         <v>4.0</v>
@@ -1782,10 +1839,19 @@
       <c r="E50" s="2">
         <v>3.0</v>
       </c>
+      <c r="F50" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="G50" s="2">
+        <v>30.0</v>
+      </c>
     </row>
     <row r="51">
+      <c r="A51" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="B51" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C51" s="2">
         <v>4.0</v>
@@ -1796,10 +1862,19 @@
       <c r="E51" s="2">
         <v>4.0</v>
       </c>
+      <c r="F51" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="G51" s="2">
+        <v>26.0</v>
+      </c>
     </row>
     <row r="52">
+      <c r="A52" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="B52" s="2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C52" s="2">
         <v>4.0</v>
@@ -1810,10 +1885,19 @@
       <c r="E52" s="2">
         <v>5.0</v>
       </c>
+      <c r="F52" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G52" s="2">
+        <v>21.0</v>
+      </c>
     </row>
     <row r="53">
+      <c r="A53" s="5" t="s">
+        <v>112</v>
+      </c>
       <c r="B53" s="2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C53" s="2">
         <v>4.0</v>
@@ -1824,10 +1908,19 @@
       <c r="E53" s="2">
         <v>6.0</v>
       </c>
+      <c r="F53" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="G53" s="2">
+        <v>16.0</v>
+      </c>
     </row>
     <row r="54">
+      <c r="A54" s="5" t="s">
+        <v>114</v>
+      </c>
       <c r="B54" s="2" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C54" s="2">
         <v>4.0</v>
@@ -1838,10 +1931,19 @@
       <c r="E54" s="2">
         <v>7.0</v>
       </c>
+      <c r="F54" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G54" s="2">
+        <v>15.0</v>
+      </c>
     </row>
     <row r="55">
+      <c r="A55" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="B55" s="2" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C55" s="2">
         <v>4.0</v>
@@ -1852,10 +1954,19 @@
       <c r="E55" s="2">
         <v>8.0</v>
       </c>
+      <c r="F55" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G55" s="2">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="56">
+      <c r="A56" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="B56" s="2" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C56" s="2">
         <v>4.0</v>
@@ -1866,10 +1977,19 @@
       <c r="E56" s="2">
         <v>9.0</v>
       </c>
+      <c r="F56" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="G56" s="2">
+        <v>12.0</v>
+      </c>
     </row>
     <row r="57">
+      <c r="A57" s="5" t="s">
+        <v>120</v>
+      </c>
       <c r="B57" s="2" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="C57" s="2">
         <v>4.0</v>
@@ -1879,6 +1999,12 @@
       </c>
       <c r="E57" s="2">
         <v>10.0</v>
+      </c>
+      <c r="F57" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G57" s="2">
+        <v>11.0</v>
       </c>
     </row>
     <row r="58">
@@ -1886,7 +2012,7 @@
         <v>9</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="C58" s="2">
         <v>5.0</v>
@@ -1902,6 +2028,9 @@
       </c>
       <c r="G58" s="2">
         <v>13.0</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="59">
@@ -1909,7 +2038,7 @@
         <v>9</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C59" s="2">
         <v>5.0</v>
@@ -1925,6 +2054,9 @@
       </c>
       <c r="G59" s="2">
         <v>50.0</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Two new days of earth data because why not (there are actual reasons)
</commit_message>
<xml_diff>
--- a/EMPANADA Data Files Key.xlsx
+++ b/EMPANADA Data Files Key.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="164">
   <si>
     <t>Original File Name:</t>
   </si>
@@ -385,6 +385,126 @@
   </si>
   <si>
     <t>Day5-Earth-2mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0642.MOV</t>
+  </si>
+  <si>
+    <t>Day6-Earth-1mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0643.MOV</t>
+  </si>
+  <si>
+    <t>Day6-Earth-2mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0644.MOV</t>
+  </si>
+  <si>
+    <t>Day6-Earth-3mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0645.MOV</t>
+  </si>
+  <si>
+    <t>Day6-Earth-4mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0646.MOV</t>
+  </si>
+  <si>
+    <t>Day6-Earth-5mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0647.MOV</t>
+  </si>
+  <si>
+    <t>Day6-Earth-6mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0648.MOV</t>
+  </si>
+  <si>
+    <t>Day6-Earth-7mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0649.MOV</t>
+  </si>
+  <si>
+    <t>Day6-Earth-8mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0650.MOV</t>
+  </si>
+  <si>
+    <t>Day6-Earth-9mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0651.MOV</t>
+  </si>
+  <si>
+    <t>Day6-Earth-10mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0652.MOV</t>
+  </si>
+  <si>
+    <t>Day7-Earth-1mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0653.MOV</t>
+  </si>
+  <si>
+    <t>Day7-Earth-2mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0654.MOV</t>
+  </si>
+  <si>
+    <t>Day7-Earth-3mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0655.MOV</t>
+  </si>
+  <si>
+    <t>Day7-Earth-4mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0656.MOV</t>
+  </si>
+  <si>
+    <t>Day7-Earth-5mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0657.MOV</t>
+  </si>
+  <si>
+    <t>Day7-Earth-6mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0658.MOV</t>
+  </si>
+  <si>
+    <t>Day7-Earth-7mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0659.MOV</t>
+  </si>
+  <si>
+    <t>Day7-Earth-8mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0660.MOV</t>
+  </si>
+  <si>
+    <t>Day7-Earth-9mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0661.MOV</t>
+  </si>
+  <si>
+    <t>Day7-Earth-10mms.mov</t>
   </si>
 </sst>
 </file>
@@ -1563,12 +1683,9 @@
       <c r="G38" s="2">
         <v>38.0</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="39">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1614,7 +1731,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1637,7 +1754,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1660,7 +1777,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -1683,7 +1800,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -1706,7 +1823,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -1729,7 +1846,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -1752,7 +1869,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -1775,7 +1892,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -1796,12 +1913,9 @@
       <c r="G48" s="2">
         <v>117.0</v>
       </c>
-      <c r="H48" s="2" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="49">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -1824,7 +1938,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -1847,7 +1961,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -1870,7 +1984,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -1893,7 +2007,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -1916,7 +2030,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -1939,7 +2053,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -1962,7 +2076,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -1985,7 +2099,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -2029,15 +2143,12 @@
       <c r="G58" s="2">
         <v>13.0</v>
       </c>
-      <c r="H58" s="2" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C59" s="2">
@@ -2055,8 +2166,465 @@
       <c r="G59" s="2">
         <v>50.0</v>
       </c>
-      <c r="H59" s="2" t="s">
-        <v>30</v>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C60" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F60" s="2">
+        <v>19.0</v>
+      </c>
+      <c r="G60" s="2">
+        <v>118.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C61" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F61" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="G61" s="2">
+        <v>54.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="F62" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G62" s="2">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="F63" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="G63" s="2">
+        <v>30.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C64" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="F64" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G64" s="2">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="F65" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="G65" s="2">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="F66" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G66" s="2">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C67" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="F67" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G67" s="2">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C68" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="F68" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G68" s="2">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C69" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="F69" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G69" s="2">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C70" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F70" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="G70" s="2">
+        <v>119.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C71" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F71" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="G71" s="2">
+        <v>54.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C72" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="F72" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G72" s="5">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C73" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="F73" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G73" s="2">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C74" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="F74" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G74" s="2">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C75" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="F75" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G75" s="2">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C76" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="F76" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="G76" s="2">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C77" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="F77" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="G77" s="2">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C78" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="F78" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G78" s="2">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C79" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="F79" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G79" s="2">
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generated all figures again
</commit_message>
<xml_diff>
--- a/EMPANADA Data Files Key.xlsx
+++ b/EMPANADA Data Files Key.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="164">
   <si>
     <t>Original File Name:</t>
   </si>
@@ -1683,6 +1683,9 @@
       <c r="G38" s="2">
         <v>38.0</v>
       </c>
+      <c r="H38" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
@@ -1706,6 +1709,9 @@
       <c r="G39" s="2">
         <v>47.0</v>
       </c>
+      <c r="H39" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
@@ -1729,6 +1735,9 @@
       <c r="G40" s="2">
         <v>31.0</v>
       </c>
+      <c r="H40" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
@@ -1752,6 +1761,9 @@
       <c r="G41" s="2">
         <v>26.0</v>
       </c>
+      <c r="H41" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
@@ -1775,6 +1787,9 @@
       <c r="G42" s="2">
         <v>20.0</v>
       </c>
+      <c r="H42" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
@@ -1798,6 +1813,9 @@
       <c r="G43" s="2">
         <v>17.0</v>
       </c>
+      <c r="H43" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
@@ -1821,6 +1839,9 @@
       <c r="G44" s="2">
         <v>15.0</v>
       </c>
+      <c r="H44" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
@@ -1844,6 +1865,9 @@
       <c r="G45" s="2">
         <v>12.5</v>
       </c>
+      <c r="H45" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
@@ -1867,6 +1891,9 @@
       <c r="G46" s="2">
         <v>11.0</v>
       </c>
+      <c r="H46" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
@@ -1890,6 +1917,9 @@
       <c r="G47" s="2">
         <v>10.0</v>
       </c>
+      <c r="H47" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
@@ -1913,6 +1943,9 @@
       <c r="G48" s="2">
         <v>117.0</v>
       </c>
+      <c r="H48" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
@@ -1936,6 +1969,9 @@
       <c r="G49" s="2">
         <v>52.0</v>
       </c>
+      <c r="H49" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
@@ -1959,6 +1995,9 @@
       <c r="G50" s="2">
         <v>30.0</v>
       </c>
+      <c r="H50" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
@@ -1982,6 +2021,9 @@
       <c r="G51" s="2">
         <v>26.0</v>
       </c>
+      <c r="H51" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
@@ -2005,6 +2047,9 @@
       <c r="G52" s="2">
         <v>21.0</v>
       </c>
+      <c r="H52" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
@@ -2028,6 +2073,9 @@
       <c r="G53" s="2">
         <v>16.0</v>
       </c>
+      <c r="H53" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
@@ -2051,6 +2099,9 @@
       <c r="G54" s="2">
         <v>15.0</v>
       </c>
+      <c r="H54" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
@@ -2074,6 +2125,9 @@
       <c r="G55" s="2">
         <v>13.0</v>
       </c>
+      <c r="H55" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
@@ -2097,6 +2151,9 @@
       <c r="G56" s="2">
         <v>12.0</v>
       </c>
+      <c r="H56" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
@@ -2120,6 +2177,9 @@
       <c r="G57" s="2">
         <v>11.0</v>
       </c>
+      <c r="H57" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
@@ -2143,6 +2203,9 @@
       <c r="G58" s="2">
         <v>13.0</v>
       </c>
+      <c r="H58" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
@@ -2166,6 +2229,9 @@
       <c r="G59" s="2">
         <v>50.0</v>
       </c>
+      <c r="H59" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
@@ -2189,6 +2255,9 @@
       <c r="G60" s="2">
         <v>118.0</v>
       </c>
+      <c r="H60" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
@@ -2418,6 +2487,9 @@
       </c>
       <c r="G70" s="2">
         <v>119.0</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="71">

</xml_diff>

<commit_message>
Took more data (days 8-11)
</commit_message>
<xml_diff>
--- a/EMPANADA Data Files Key.xlsx
+++ b/EMPANADA Data Files Key.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="204">
   <si>
     <t>Original File Name:</t>
   </si>
@@ -505,6 +505,126 @@
   </si>
   <si>
     <t>Day7-Earth-10mms.mov</t>
+  </si>
+  <si>
+    <t>MVI_0001.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0002.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0003.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0004.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0005.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0006.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0007.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0008.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0009.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0010.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0011.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0012.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0013.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0014.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0015.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0016.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0017.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0018.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0019.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0020.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0021.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0022.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0023.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0024.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0025.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0026.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0027.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0028.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0029.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0041.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0030.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0031.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0032.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0033.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0034.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0035.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0036.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0037.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0038.MOV</t>
+  </si>
+  <si>
+    <t>MVI_0040.MOV</t>
   </si>
 </sst>
 </file>
@@ -2145,7 +2265,7 @@
       <c r="E56" s="2">
         <v>9.0</v>
       </c>
-      <c r="F56" s="5">
+      <c r="F56" s="2">
         <v>1.5</v>
       </c>
       <c r="G56" s="2">
@@ -2260,10 +2380,10 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C61" s="2">
@@ -2283,10 +2403,10 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="2" t="s">
         <v>129</v>
       </c>
       <c r="C62" s="2">
@@ -2306,10 +2426,10 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="2" t="s">
         <v>131</v>
       </c>
       <c r="C63" s="2">
@@ -2329,10 +2449,10 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="2" t="s">
         <v>133</v>
       </c>
       <c r="C64" s="2">
@@ -2352,10 +2472,10 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="2" t="s">
         <v>135</v>
       </c>
       <c r="C65" s="2">
@@ -2375,10 +2495,10 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="2" t="s">
         <v>137</v>
       </c>
       <c r="C66" s="2">
@@ -2398,10 +2518,10 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="2" t="s">
         <v>139</v>
       </c>
       <c r="C67" s="2">
@@ -2421,10 +2541,10 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="2" t="s">
         <v>141</v>
       </c>
       <c r="C68" s="2">
@@ -2444,10 +2564,10 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="2" t="s">
         <v>143</v>
       </c>
       <c r="C69" s="2">
@@ -2467,10 +2587,10 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="2" t="s">
         <v>145</v>
       </c>
       <c r="C70" s="2">
@@ -2493,10 +2613,10 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="5" t="s">
+      <c r="A71" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="2" t="s">
         <v>147</v>
       </c>
       <c r="C71" s="2">
@@ -2516,10 +2636,10 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C72" s="2">
@@ -2534,15 +2654,15 @@
       <c r="F72" s="2">
         <v>2.0</v>
       </c>
-      <c r="G72" s="5">
+      <c r="G72" s="2">
         <v>35.0</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="2" t="s">
         <v>151</v>
       </c>
       <c r="C73" s="2">
@@ -2562,10 +2682,10 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="2" t="s">
         <v>153</v>
       </c>
       <c r="C74" s="2">
@@ -2585,10 +2705,10 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="5" t="s">
+      <c r="A75" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="2" t="s">
         <v>155</v>
       </c>
       <c r="C75" s="2">
@@ -2608,10 +2728,10 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="2" t="s">
         <v>157</v>
       </c>
       <c r="C76" s="2">
@@ -2631,10 +2751,10 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="5" t="s">
+      <c r="A77" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="2" t="s">
         <v>159</v>
       </c>
       <c r="C77" s="2">
@@ -2654,10 +2774,10 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C78" s="2">
@@ -2677,10 +2797,10 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="2" t="s">
         <v>163</v>
       </c>
       <c r="C79" s="2">
@@ -2696,6 +2816,726 @@
         <v>0.0</v>
       </c>
       <c r="G79" s="2">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B80" s="3" t="str">
+        <f t="shared" ref="B80:B119" si="2">"Day"&amp;C80&amp;"-"&amp;D80&amp;"-"&amp;E80&amp;"mms.mov"</f>
+        <v>Day8-Earth-1mms.mov</v>
+      </c>
+      <c r="C80" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day8-Earth-2mms.mov</v>
+      </c>
+      <c r="C81" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B82" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day8-Earth-3mms.mov</v>
+      </c>
+      <c r="C82" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B83" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day8-Earth-4mms.mov</v>
+      </c>
+      <c r="C83" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" s="2">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B84" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day8-Earth-5mms.mov</v>
+      </c>
+      <c r="C84" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" s="2">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B85" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day8-Earth-6mms.mov</v>
+      </c>
+      <c r="C85" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" s="2">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day8-Earth-7mms.mov</v>
+      </c>
+      <c r="C86" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86" s="2">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B87" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day8-Earth-8mms.mov</v>
+      </c>
+      <c r="C87" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" s="2">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B88" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day8-Earth-9mms.mov</v>
+      </c>
+      <c r="C88" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E88" s="2">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B89" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day8-Earth-10mms.mov</v>
+      </c>
+      <c r="C89" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" s="2">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B90" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day9-Earth-1mms.mov</v>
+      </c>
+      <c r="C90" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E90" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B91" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day9-Earth-2mms.mov</v>
+      </c>
+      <c r="C91" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E91" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B92" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day9-Earth-3mms.mov</v>
+      </c>
+      <c r="C92" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E92" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B93" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day9-Earth-4mms.mov</v>
+      </c>
+      <c r="C93" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E93" s="2">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B94" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day9-Earth-5mms.mov</v>
+      </c>
+      <c r="C94" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E94" s="2">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B95" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day9-Earth-6mms.mov</v>
+      </c>
+      <c r="C95" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E95" s="2">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B96" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day9-Earth-7mms.mov</v>
+      </c>
+      <c r="C96" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E96" s="2">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B97" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day9-Earth-8mms.mov</v>
+      </c>
+      <c r="C97" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E97" s="2">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B98" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day9-Earth-9mms.mov</v>
+      </c>
+      <c r="C98" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E98" s="2">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B99" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day9-Earth-10mms.mov</v>
+      </c>
+      <c r="C99" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E99" s="2">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B100" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day10-Earth-1mms.mov</v>
+      </c>
+      <c r="C100" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E100" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B101" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day10-Earth-2mms.mov</v>
+      </c>
+      <c r="C101" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E101" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B102" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day10-Earth-3mms.mov</v>
+      </c>
+      <c r="C102" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E102" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B103" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day10-Earth-4mms.mov</v>
+      </c>
+      <c r="C103" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E103" s="2">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B104" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day10-Earth-5mms.mov</v>
+      </c>
+      <c r="C104" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E104" s="2">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B105" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day10-Earth-6mms.mov</v>
+      </c>
+      <c r="C105" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E105" s="2">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B106" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day10-Earth-7mms.mov</v>
+      </c>
+      <c r="C106" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E106" s="2">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B107" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day10-Earth-8mms.mov</v>
+      </c>
+      <c r="C107" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E107" s="2">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B108" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day10-Earth-9mms.mov</v>
+      </c>
+      <c r="C108" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E108" s="2">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B109" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day10-Earth-10mms.mov</v>
+      </c>
+      <c r="C109" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E109" s="2">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B110" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day11-Earth-1mms.mov</v>
+      </c>
+      <c r="C110" s="5">
+        <v>11.0</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E110" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B111" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day11-Earth-2mms.mov</v>
+      </c>
+      <c r="C111" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E111" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B112" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day11-Earth-3mms.mov</v>
+      </c>
+      <c r="C112" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E112" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B113" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day11-Earth-4mms.mov</v>
+      </c>
+      <c r="C113" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E113" s="2">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B114" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day11-Earth-5mms.mov</v>
+      </c>
+      <c r="C114" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E114" s="2">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B115" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day11-Earth-6mms.mov</v>
+      </c>
+      <c r="C115" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E115" s="2">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B116" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day11-Earth-7mms.mov</v>
+      </c>
+      <c r="C116" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E116" s="2">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B117" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day11-Earth-8mms.mov</v>
+      </c>
+      <c r="C117" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E117" s="2">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B118" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day11-Earth-9mms.mov</v>
+      </c>
+      <c r="C118" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E118" s="2">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B119" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Day11-Earth-10mms.mov</v>
+      </c>
+      <c r="C119" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E119" s="2">
         <v>10.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Analyzed new data and generated max load figures
</commit_message>
<xml_diff>
--- a/EMPANADA Data Files Key.xlsx
+++ b/EMPANADA Data Files Key.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="204">
   <si>
     <t>Original File Name:</t>
   </si>
@@ -2401,6 +2401,9 @@
       <c r="G61" s="2">
         <v>54.0</v>
       </c>
+      <c r="H61" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
@@ -2424,6 +2427,9 @@
       <c r="G62" s="2">
         <v>35.0</v>
       </c>
+      <c r="H62" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
@@ -2447,6 +2453,9 @@
       <c r="G63" s="2">
         <v>30.0</v>
       </c>
+      <c r="H63" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
@@ -2470,6 +2479,9 @@
       <c r="G64" s="2">
         <v>21.0</v>
       </c>
+      <c r="H64" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
@@ -2493,6 +2505,9 @@
       <c r="G65" s="2">
         <v>21.0</v>
       </c>
+      <c r="H65" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
@@ -2516,6 +2531,9 @@
       <c r="G66" s="2">
         <v>15.0</v>
       </c>
+      <c r="H66" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
@@ -2539,6 +2557,9 @@
       <c r="G67" s="2">
         <v>13.0</v>
       </c>
+      <c r="H67" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
@@ -2562,6 +2583,9 @@
       <c r="G68" s="2">
         <v>11.5</v>
       </c>
+      <c r="H68" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
@@ -2585,6 +2609,9 @@
       <c r="G69" s="2">
         <v>12.0</v>
       </c>
+      <c r="H69" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
@@ -2608,7 +2635,7 @@
       <c r="G70" s="2">
         <v>119.0</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="H70" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2634,6 +2661,9 @@
       <c r="G71" s="2">
         <v>54.0</v>
       </c>
+      <c r="H71" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="s">
@@ -2657,6 +2687,9 @@
       <c r="G72" s="2">
         <v>35.0</v>
       </c>
+      <c r="H72" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="s">
@@ -2680,6 +2713,9 @@
       <c r="G73" s="2">
         <v>27.0</v>
       </c>
+      <c r="H73" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="s">
@@ -2703,6 +2739,9 @@
       <c r="G74" s="2">
         <v>21.0</v>
       </c>
+      <c r="H74" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="s">
@@ -2726,6 +2765,9 @@
       <c r="G75" s="2">
         <v>17.0</v>
       </c>
+      <c r="H75" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
@@ -2743,11 +2785,14 @@
       <c r="E76" s="2">
         <v>7.0</v>
       </c>
-      <c r="F76" s="5">
+      <c r="F76" s="2">
         <v>0.0</v>
       </c>
       <c r="G76" s="2">
         <v>14.0</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="77">
@@ -2772,6 +2817,9 @@
       <c r="G77" s="2">
         <v>15.5</v>
       </c>
+      <c r="H77" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="s">
@@ -2795,6 +2843,9 @@
       <c r="G78" s="2">
         <v>11.0</v>
       </c>
+      <c r="H78" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="s">
@@ -2818,6 +2869,9 @@
       <c r="G79" s="2">
         <v>10.0</v>
       </c>
+      <c r="H79" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="s">
@@ -2827,7 +2881,7 @@
         <f t="shared" ref="B80:B119" si="2">"Day"&amp;C80&amp;"-"&amp;D80&amp;"-"&amp;E80&amp;"mms.mov"</f>
         <v>Day8-Earth-1mms.mov</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C80" s="2">
         <v>8.0</v>
       </c>
       <c r="D80" s="2" t="s">
@@ -2836,9 +2890,18 @@
       <c r="E80" s="2">
         <v>1.0</v>
       </c>
+      <c r="F80" s="2">
+        <v>13.0</v>
+      </c>
+      <c r="G80" s="2">
+        <v>137.0</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="81">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="2" t="s">
         <v>165</v>
       </c>
       <c r="B81" s="3" t="str">
@@ -2854,6 +2917,12 @@
       <c r="E81" s="2">
         <v>2.0</v>
       </c>
+      <c r="F81" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G81" s="2">
+        <v>63.0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="s">
@@ -2872,9 +2941,15 @@
       <c r="E82" s="2">
         <v>3.0</v>
       </c>
+      <c r="F82" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G82" s="2">
+        <v>41.0</v>
+      </c>
     </row>
     <row r="83">
-      <c r="A83" s="5" t="s">
+      <c r="A83" s="2" t="s">
         <v>167</v>
       </c>
       <c r="B83" s="3" t="str">
@@ -2890,9 +2965,15 @@
       <c r="E83" s="2">
         <v>4.0</v>
       </c>
+      <c r="F83" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G83" s="2">
+        <v>30.0</v>
+      </c>
     </row>
     <row r="84">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B84" s="3" t="str">
@@ -2908,9 +2989,15 @@
       <c r="E84" s="2">
         <v>5.0</v>
       </c>
+      <c r="F84" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G84" s="2">
+        <v>26.0</v>
+      </c>
     </row>
     <row r="85">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="2" t="s">
         <v>169</v>
       </c>
       <c r="B85" s="3" t="str">
@@ -2926,9 +3013,15 @@
       <c r="E85" s="2">
         <v>6.0</v>
       </c>
+      <c r="F85" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="G85" s="2">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="86">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="2" t="s">
         <v>170</v>
       </c>
       <c r="B86" s="3" t="str">
@@ -2944,9 +3037,15 @@
       <c r="E86" s="2">
         <v>7.0</v>
       </c>
+      <c r="F86" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G86" s="2">
+        <v>19.0</v>
+      </c>
     </row>
     <row r="87">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="2" t="s">
         <v>171</v>
       </c>
       <c r="B87" s="3" t="str">
@@ -2962,9 +3061,15 @@
       <c r="E87" s="2">
         <v>8.0</v>
       </c>
+      <c r="F87" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="G87" s="2">
+        <v>18.0</v>
+      </c>
     </row>
     <row r="88">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B88" s="3" t="str">
@@ -2980,9 +3085,15 @@
       <c r="E88" s="2">
         <v>9.0</v>
       </c>
+      <c r="F88" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G88" s="2">
+        <v>16.0</v>
+      </c>
     </row>
     <row r="89">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="2" t="s">
         <v>173</v>
       </c>
       <c r="B89" s="3" t="str">
@@ -2998,9 +3109,15 @@
       <c r="E89" s="2">
         <v>10.0</v>
       </c>
+      <c r="F89" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="G89" s="2">
+        <v>14.0</v>
+      </c>
     </row>
     <row r="90">
-      <c r="A90" s="5" t="s">
+      <c r="A90" s="2" t="s">
         <v>174</v>
       </c>
       <c r="B90" s="3" t="str">
@@ -3016,9 +3133,18 @@
       <c r="E90" s="2">
         <v>1.0</v>
       </c>
+      <c r="F90" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="G90" s="2">
+        <v>135.0</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="91">
-      <c r="A91" s="5" t="s">
+      <c r="A91" s="2" t="s">
         <v>175</v>
       </c>
       <c r="B91" s="3" t="str">
@@ -3034,9 +3160,15 @@
       <c r="E91" s="2">
         <v>2.0</v>
       </c>
+      <c r="F91" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G91" s="2">
+        <v>62.0</v>
+      </c>
     </row>
     <row r="92">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B92" s="3" t="str">
@@ -3052,9 +3184,15 @@
       <c r="E92" s="2">
         <v>3.0</v>
       </c>
+      <c r="F92" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G92" s="2">
+        <v>40.0</v>
+      </c>
     </row>
     <row r="93">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="2" t="s">
         <v>177</v>
       </c>
       <c r="B93" s="3" t="str">
@@ -3070,9 +3208,15 @@
       <c r="E93" s="2">
         <v>4.0</v>
       </c>
+      <c r="F93" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="G93" s="2">
+        <v>33.0</v>
+      </c>
     </row>
     <row r="94">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B94" s="3" t="str">
@@ -3088,9 +3232,15 @@
       <c r="E94" s="2">
         <v>5.0</v>
       </c>
+      <c r="F94" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G94" s="2">
+        <v>26.0</v>
+      </c>
     </row>
     <row r="95">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="2" t="s">
         <v>179</v>
       </c>
       <c r="B95" s="3" t="str">
@@ -3106,9 +3256,15 @@
       <c r="E95" s="2">
         <v>6.0</v>
       </c>
+      <c r="F95" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G95" s="2">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="96">
-      <c r="A96" s="5" t="s">
+      <c r="A96" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B96" s="3" t="str">
@@ -3124,9 +3280,15 @@
       <c r="E96" s="2">
         <v>7.0</v>
       </c>
+      <c r="F96" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="G96" s="2">
+        <v>19.0</v>
+      </c>
     </row>
     <row r="97">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B97" s="3" t="str">
@@ -3142,9 +3304,15 @@
       <c r="E97" s="2">
         <v>8.0</v>
       </c>
+      <c r="F97" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="G97" s="2">
+        <v>17.0</v>
+      </c>
     </row>
     <row r="98">
-      <c r="A98" s="5" t="s">
+      <c r="A98" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B98" s="3" t="str">
@@ -3160,9 +3328,15 @@
       <c r="E98" s="2">
         <v>9.0</v>
       </c>
+      <c r="F98" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G98" s="5">
+        <v>16.0</v>
+      </c>
     </row>
     <row r="99">
-      <c r="A99" s="5" t="s">
+      <c r="A99" s="2" t="s">
         <v>183</v>
       </c>
       <c r="B99" s="3" t="str">
@@ -3178,9 +3352,15 @@
       <c r="E99" s="2">
         <v>10.0</v>
       </c>
+      <c r="F99" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G99" s="2">
+        <v>13.5</v>
+      </c>
     </row>
     <row r="100">
-      <c r="A100" s="5" t="s">
+      <c r="A100" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B100" s="3" t="str">
@@ -3196,9 +3376,18 @@
       <c r="E100" s="2">
         <v>1.0</v>
       </c>
+      <c r="F100" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="G100" s="2">
+        <v>140.0</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="101">
-      <c r="A101" s="5" t="s">
+      <c r="A101" s="2" t="s">
         <v>185</v>
       </c>
       <c r="B101" s="3" t="str">
@@ -3214,9 +3403,15 @@
       <c r="E101" s="2">
         <v>2.0</v>
       </c>
+      <c r="F101" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G101" s="2">
+        <v>65.0</v>
+      </c>
     </row>
     <row r="102">
-      <c r="A102" s="5" t="s">
+      <c r="A102" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B102" s="3" t="str">
@@ -3232,9 +3427,15 @@
       <c r="E102" s="2">
         <v>3.0</v>
       </c>
+      <c r="F102" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G102" s="2">
+        <v>43.0</v>
+      </c>
     </row>
     <row r="103">
-      <c r="A103" s="5" t="s">
+      <c r="A103" s="2" t="s">
         <v>187</v>
       </c>
       <c r="B103" s="3" t="str">
@@ -3250,9 +3451,15 @@
       <c r="E103" s="2">
         <v>4.0</v>
       </c>
+      <c r="F103" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G103" s="2">
+        <v>35.0</v>
+      </c>
     </row>
     <row r="104">
-      <c r="A104" s="5" t="s">
+      <c r="A104" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B104" s="3" t="str">
@@ -3268,9 +3475,15 @@
       <c r="E104" s="2">
         <v>5.0</v>
       </c>
+      <c r="F104" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="G104" s="2">
+        <v>28.0</v>
+      </c>
     </row>
     <row r="105">
-      <c r="A105" s="5" t="s">
+      <c r="A105" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B105" s="3" t="str">
@@ -3286,9 +3499,15 @@
       <c r="E105" s="2">
         <v>6.0</v>
       </c>
+      <c r="F105" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G105" s="2">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="106">
-      <c r="A106" s="5" t="s">
+      <c r="A106" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B106" s="3" t="str">
@@ -3304,9 +3523,15 @@
       <c r="E106" s="2">
         <v>7.0</v>
       </c>
+      <c r="F106" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G106" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="107">
-      <c r="A107" s="5" t="s">
+      <c r="A107" s="2" t="s">
         <v>191</v>
       </c>
       <c r="B107" s="3" t="str">
@@ -3322,9 +3547,15 @@
       <c r="E107" s="2">
         <v>8.0</v>
       </c>
+      <c r="F107" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G107" s="2">
+        <v>17.0</v>
+      </c>
     </row>
     <row r="108">
-      <c r="A108" s="5" t="s">
+      <c r="A108" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B108" s="3" t="str">
@@ -3340,6 +3571,12 @@
       <c r="E108" s="2">
         <v>9.0</v>
       </c>
+      <c r="F108" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G108" s="2">
+        <v>15.0</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="s">
@@ -3358,16 +3595,22 @@
       <c r="E109" s="2">
         <v>10.0</v>
       </c>
+      <c r="F109" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G109" s="2">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="110">
-      <c r="A110" s="5" t="s">
+      <c r="A110" s="2" t="s">
         <v>194</v>
       </c>
       <c r="B110" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Day11-Earth-1mms.mov</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C110" s="2">
         <v>11.0</v>
       </c>
       <c r="D110" s="2" t="s">
@@ -3376,9 +3619,18 @@
       <c r="E110" s="2">
         <v>1.0</v>
       </c>
+      <c r="F110" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G110" s="2">
+        <v>140.0</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="111">
-      <c r="A111" s="5" t="s">
+      <c r="A111" s="2" t="s">
         <v>195</v>
       </c>
       <c r="B111" s="3" t="str">
@@ -3394,9 +3646,15 @@
       <c r="E111" s="2">
         <v>2.0</v>
       </c>
+      <c r="F111" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G111" s="2">
+        <v>67.0</v>
+      </c>
     </row>
     <row r="112">
-      <c r="A112" s="5" t="s">
+      <c r="A112" s="2" t="s">
         <v>196</v>
       </c>
       <c r="B112" s="3" t="str">
@@ -3412,9 +3670,15 @@
       <c r="E112" s="2">
         <v>3.0</v>
       </c>
+      <c r="F112" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G112" s="2">
+        <v>44.0</v>
+      </c>
     </row>
     <row r="113">
-      <c r="A113" s="5" t="s">
+      <c r="A113" s="2" t="s">
         <v>197</v>
       </c>
       <c r="B113" s="3" t="str">
@@ -3430,9 +3694,15 @@
       <c r="E113" s="2">
         <v>4.0</v>
       </c>
+      <c r="F113" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G113" s="2">
+        <v>33.0</v>
+      </c>
     </row>
     <row r="114">
-      <c r="A114" s="5" t="s">
+      <c r="A114" s="2" t="s">
         <v>198</v>
       </c>
       <c r="B114" s="3" t="str">
@@ -3448,9 +3718,15 @@
       <c r="E114" s="2">
         <v>5.0</v>
       </c>
+      <c r="F114" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G114" s="2">
+        <v>26.0</v>
+      </c>
     </row>
     <row r="115">
-      <c r="A115" s="5" t="s">
+      <c r="A115" s="2" t="s">
         <v>199</v>
       </c>
       <c r="B115" s="3" t="str">
@@ -3466,9 +3742,15 @@
       <c r="E115" s="2">
         <v>6.0</v>
       </c>
+      <c r="F115" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G115" s="2">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="116">
-      <c r="A116" s="5" t="s">
+      <c r="A116" s="2" t="s">
         <v>200</v>
       </c>
       <c r="B116" s="3" t="str">
@@ -3484,9 +3766,15 @@
       <c r="E116" s="2">
         <v>7.0</v>
       </c>
+      <c r="F116" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G116" s="2">
+        <v>19.0</v>
+      </c>
     </row>
     <row r="117">
-      <c r="A117" s="5" t="s">
+      <c r="A117" s="2" t="s">
         <v>201</v>
       </c>
       <c r="B117" s="3" t="str">
@@ -3502,9 +3790,15 @@
       <c r="E117" s="2">
         <v>8.0</v>
       </c>
+      <c r="F117" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G117" s="2">
+        <v>17.0</v>
+      </c>
     </row>
     <row r="118">
-      <c r="A118" s="5" t="s">
+      <c r="A118" s="2" t="s">
         <v>202</v>
       </c>
       <c r="B118" s="3" t="str">
@@ -3520,6 +3814,12 @@
       <c r="E118" s="2">
         <v>9.0</v>
       </c>
+      <c r="F118" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G118" s="2">
+        <v>15.5</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="s">
@@ -3537,6 +3837,12 @@
       </c>
       <c r="E119" s="2">
         <v>10.0</v>
+      </c>
+      <c r="F119" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="G119" s="2">
+        <v>14.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Whole bunch of stuff, I forgot to commit for a while: added most outputs to gitignore, updated G squared method and ran it several times, Data files key now has most entries as active, updated method comparison and made it compare G squared as well as brightness and force, probably some other stuff too...
</commit_message>
<xml_diff>
--- a/EMPANADA Data Files Key.xlsx
+++ b/EMPANADA Data Files Key.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="204">
   <si>
     <t>Original File Name:</t>
   </si>
@@ -631,7 +631,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -650,7 +650,6 @@
       <color theme="1"/>
       <name val="Serif"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -666,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -678,9 +677,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -972,6 +968,10 @@
       <c r="G3" s="2">
         <v>32.0</v>
       </c>
+      <c r="I3" s="3">
+        <f t="shared" ref="I3:I119" si="1">G3-F3</f>
+        <v>28</v>
+      </c>
       <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
@@ -998,6 +998,10 @@
       <c r="G4" s="2">
         <v>20.0</v>
       </c>
+      <c r="I4" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
       <c r="J4" s="2" t="s">
         <v>17</v>
       </c>
@@ -1024,6 +1028,10 @@
       <c r="G5" s="2">
         <v>27.0</v>
       </c>
+      <c r="I5" s="3">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
@@ -1047,6 +1055,10 @@
       <c r="G6" s="4">
         <v>42.0</v>
       </c>
+      <c r="I6" s="3">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
@@ -1070,6 +1082,10 @@
       <c r="G7" s="4">
         <v>18.5</v>
       </c>
+      <c r="I7" s="3">
+        <f t="shared" si="1"/>
+        <v>9.5</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
@@ -1093,6 +1109,10 @@
       <c r="G8" s="2">
         <v>42.0</v>
       </c>
+      <c r="I8" s="3">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
@@ -1119,6 +1139,10 @@
       <c r="H9" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="I9" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
@@ -1145,6 +1169,10 @@
       <c r="H10" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="I10" s="3">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
@@ -1168,6 +1196,10 @@
       <c r="G11" s="2">
         <v>28.0</v>
       </c>
+      <c r="I11" s="3">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
@@ -1191,6 +1223,10 @@
       <c r="G12" s="2">
         <v>24.0</v>
       </c>
+      <c r="I12" s="3">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
@@ -1214,6 +1250,10 @@
       <c r="G13" s="2">
         <v>35.0</v>
       </c>
+      <c r="I13" s="3">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
@@ -1237,6 +1277,10 @@
       <c r="G14" s="2">
         <v>19.0</v>
       </c>
+      <c r="I14" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
@@ -1260,6 +1304,10 @@
       <c r="G15" s="2">
         <v>30.0</v>
       </c>
+      <c r="I15" s="3">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
@@ -1283,6 +1331,10 @@
       <c r="G16" s="2">
         <v>21.0</v>
       </c>
+      <c r="I16" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
@@ -1306,6 +1358,10 @@
       <c r="G17" s="2">
         <v>20.0</v>
       </c>
+      <c r="I17" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
@@ -1332,6 +1388,10 @@
       <c r="H18" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="I18" s="3">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
@@ -1355,6 +1415,10 @@
       <c r="G19" s="2">
         <v>20.0</v>
       </c>
+      <c r="I19" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
@@ -1378,6 +1442,10 @@
       <c r="G20" s="2">
         <v>26.0</v>
       </c>
+      <c r="I20" s="3">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
@@ -1401,6 +1469,10 @@
       <c r="G21" s="2">
         <v>27.0</v>
       </c>
+      <c r="I21" s="3">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
@@ -1424,6 +1496,10 @@
       <c r="G22" s="2">
         <v>22.0</v>
       </c>
+      <c r="I22" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
@@ -1450,6 +1526,10 @@
       <c r="H23" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="I23" s="3">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
@@ -1473,6 +1553,10 @@
       <c r="G24" s="2">
         <v>19.0</v>
       </c>
+      <c r="I24" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
@@ -1496,6 +1580,10 @@
       <c r="G25" s="2">
         <v>30.0</v>
       </c>
+      <c r="I25" s="3">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
@@ -1519,6 +1607,10 @@
       <c r="G26" s="2">
         <v>21.0</v>
       </c>
+      <c r="I26" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
@@ -1542,6 +1634,10 @@
       <c r="G27" s="2">
         <v>20.0</v>
       </c>
+      <c r="I27" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
@@ -1568,6 +1664,10 @@
       <c r="H28" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="I28" s="3">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
@@ -1591,6 +1691,10 @@
       <c r="G29" s="2">
         <v>19.0</v>
       </c>
+      <c r="I29" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
@@ -1614,6 +1718,10 @@
       <c r="G30" s="2">
         <v>24.0</v>
       </c>
+      <c r="I30" s="3">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
@@ -1637,6 +1745,10 @@
       <c r="G31" s="2">
         <v>26.0</v>
       </c>
+      <c r="I31" s="3">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
@@ -1660,13 +1772,17 @@
       <c r="G32" s="2">
         <v>22.0</v>
       </c>
+      <c r="I32" s="3">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B33" s="3" t="str">
-        <f t="shared" ref="B33:B37" si="1">"Day"&amp;C33&amp;"-"&amp;D33&amp;"-"&amp;E33&amp;"mms.mov"</f>
+        <f t="shared" ref="B33:B37" si="2">"Day"&amp;C33&amp;"-"&amp;D33&amp;"-"&amp;E33&amp;"mms.mov"</f>
         <v>Day2-Martian-70mms.mov</v>
       </c>
       <c r="C33" s="2">
@@ -1683,6 +1799,10 @@
       </c>
       <c r="G33" s="2">
         <v>33.0</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
     </row>
     <row r="34">
@@ -1690,7 +1810,7 @@
         <v>78</v>
       </c>
       <c r="B34" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Day2-Martian-210mms.mov</v>
       </c>
       <c r="C34" s="2">
@@ -1707,6 +1827,10 @@
       </c>
       <c r="G34" s="2">
         <v>19.0</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
     </row>
     <row r="35">
@@ -1714,7 +1838,7 @@
         <v>79</v>
       </c>
       <c r="B35" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Day2-Martian-130mms.mov</v>
       </c>
       <c r="C35" s="2">
@@ -1731,6 +1855,10 @@
       </c>
       <c r="G35" s="2">
         <v>26.0</v>
+      </c>
+      <c r="I35" s="3">
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
     </row>
     <row r="36">
@@ -1738,7 +1866,7 @@
         <v>80</v>
       </c>
       <c r="B36" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Day2-Lunar-70mms.mov</v>
       </c>
       <c r="C36" s="2">
@@ -1755,6 +1883,10 @@
       </c>
       <c r="G36" s="4">
         <v>41.0</v>
+      </c>
+      <c r="I36" s="3">
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
     </row>
     <row r="37">
@@ -1762,7 +1894,7 @@
         <v>81</v>
       </c>
       <c r="B37" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Day2-Lunar-210mms.mov</v>
       </c>
       <c r="C37" s="2">
@@ -1779,6 +1911,10 @@
       </c>
       <c r="G37" s="4">
         <v>18.5</v>
+      </c>
+      <c r="I37" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
     </row>
     <row r="38">
@@ -1803,8 +1939,9 @@
       <c r="G38" s="2">
         <v>38.0</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>30</v>
+      <c r="I38" s="3">
+        <f t="shared" si="1"/>
+        <v>36</v>
       </c>
     </row>
     <row r="39">
@@ -1829,8 +1966,9 @@
       <c r="G39" s="2">
         <v>47.0</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>30</v>
+      <c r="I39" s="3">
+        <f t="shared" si="1"/>
+        <v>43</v>
       </c>
     </row>
     <row r="40">
@@ -1855,8 +1993,9 @@
       <c r="G40" s="2">
         <v>31.0</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>30</v>
+      <c r="I40" s="3">
+        <f t="shared" si="1"/>
+        <v>28</v>
       </c>
     </row>
     <row r="41">
@@ -1881,8 +2020,9 @@
       <c r="G41" s="2">
         <v>26.0</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>30</v>
+      <c r="I41" s="3">
+        <f t="shared" si="1"/>
+        <v>23</v>
       </c>
     </row>
     <row r="42">
@@ -1907,8 +2047,9 @@
       <c r="G42" s="2">
         <v>20.0</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>30</v>
+      <c r="I42" s="3">
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
     </row>
     <row r="43">
@@ -1933,8 +2074,9 @@
       <c r="G43" s="2">
         <v>17.0</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>30</v>
+      <c r="I43" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="44">
@@ -1959,8 +2101,9 @@
       <c r="G44" s="2">
         <v>15.0</v>
       </c>
-      <c r="H44" s="2" t="s">
-        <v>30</v>
+      <c r="I44" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="45">
@@ -1985,8 +2128,9 @@
       <c r="G45" s="2">
         <v>12.5</v>
       </c>
-      <c r="H45" s="2" t="s">
-        <v>30</v>
+      <c r="I45" s="3">
+        <f t="shared" si="1"/>
+        <v>11.5</v>
       </c>
     </row>
     <row r="46">
@@ -2011,8 +2155,9 @@
       <c r="G46" s="2">
         <v>11.0</v>
       </c>
-      <c r="H46" s="2" t="s">
-        <v>30</v>
+      <c r="I46" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="47">
@@ -2037,8 +2182,9 @@
       <c r="G47" s="2">
         <v>10.0</v>
       </c>
-      <c r="H47" s="2" t="s">
-        <v>30</v>
+      <c r="I47" s="3">
+        <f t="shared" si="1"/>
+        <v>9.5</v>
       </c>
     </row>
     <row r="48">
@@ -2063,8 +2209,9 @@
       <c r="G48" s="2">
         <v>117.0</v>
       </c>
-      <c r="H48" s="2" t="s">
-        <v>30</v>
+      <c r="I48" s="3">
+        <f t="shared" si="1"/>
+        <v>96</v>
       </c>
     </row>
     <row r="49">
@@ -2089,8 +2236,9 @@
       <c r="G49" s="2">
         <v>52.0</v>
       </c>
-      <c r="H49" s="2" t="s">
-        <v>30</v>
+      <c r="I49" s="3">
+        <f t="shared" si="1"/>
+        <v>37</v>
       </c>
     </row>
     <row r="50">
@@ -2115,8 +2263,9 @@
       <c r="G50" s="2">
         <v>30.0</v>
       </c>
-      <c r="H50" s="2" t="s">
-        <v>30</v>
+      <c r="I50" s="3">
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
     </row>
     <row r="51">
@@ -2141,8 +2290,9 @@
       <c r="G51" s="2">
         <v>26.0</v>
       </c>
-      <c r="H51" s="2" t="s">
-        <v>30</v>
+      <c r="I51" s="3">
+        <f t="shared" si="1"/>
+        <v>23</v>
       </c>
     </row>
     <row r="52">
@@ -2167,8 +2317,9 @@
       <c r="G52" s="2">
         <v>21.0</v>
       </c>
-      <c r="H52" s="2" t="s">
-        <v>30</v>
+      <c r="I52" s="3">
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
     </row>
     <row r="53">
@@ -2193,8 +2344,9 @@
       <c r="G53" s="2">
         <v>16.0</v>
       </c>
-      <c r="H53" s="2" t="s">
-        <v>30</v>
+      <c r="I53" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
     </row>
     <row r="54">
@@ -2219,8 +2371,9 @@
       <c r="G54" s="2">
         <v>15.0</v>
       </c>
-      <c r="H54" s="2" t="s">
-        <v>30</v>
+      <c r="I54" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="55">
@@ -2245,8 +2398,9 @@
       <c r="G55" s="2">
         <v>13.0</v>
       </c>
-      <c r="H55" s="2" t="s">
-        <v>30</v>
+      <c r="I55" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
     </row>
     <row r="56">
@@ -2271,8 +2425,9 @@
       <c r="G56" s="2">
         <v>12.0</v>
       </c>
-      <c r="H56" s="2" t="s">
-        <v>30</v>
+      <c r="I56" s="3">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
       </c>
     </row>
     <row r="57">
@@ -2297,8 +2452,9 @@
       <c r="G57" s="2">
         <v>11.0</v>
       </c>
-      <c r="H57" s="2" t="s">
-        <v>30</v>
+      <c r="I57" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
     </row>
     <row r="58">
@@ -2326,6 +2482,10 @@
       <c r="H58" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="I58" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
@@ -2352,6 +2512,10 @@
       <c r="H59" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="I59" s="3">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
@@ -2375,8 +2539,9 @@
       <c r="G60" s="2">
         <v>118.0</v>
       </c>
-      <c r="H60" s="2" t="s">
-        <v>30</v>
+      <c r="I60" s="3">
+        <f t="shared" si="1"/>
+        <v>99</v>
       </c>
     </row>
     <row r="61">
@@ -2401,8 +2566,9 @@
       <c r="G61" s="2">
         <v>54.0</v>
       </c>
-      <c r="H61" s="2" t="s">
-        <v>30</v>
+      <c r="I61" s="3">
+        <f t="shared" si="1"/>
+        <v>51</v>
       </c>
     </row>
     <row r="62">
@@ -2427,8 +2593,9 @@
       <c r="G62" s="2">
         <v>35.0</v>
       </c>
-      <c r="H62" s="2" t="s">
-        <v>30</v>
+      <c r="I62" s="3">
+        <f t="shared" si="1"/>
+        <v>34</v>
       </c>
     </row>
     <row r="63">
@@ -2453,8 +2620,9 @@
       <c r="G63" s="2">
         <v>30.0</v>
       </c>
-      <c r="H63" s="2" t="s">
-        <v>30</v>
+      <c r="I63" s="3">
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
     </row>
     <row r="64">
@@ -2479,8 +2647,9 @@
       <c r="G64" s="2">
         <v>21.0</v>
       </c>
-      <c r="H64" s="2" t="s">
-        <v>30</v>
+      <c r="I64" s="3">
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
     </row>
     <row r="65">
@@ -2505,8 +2674,9 @@
       <c r="G65" s="2">
         <v>21.0</v>
       </c>
-      <c r="H65" s="2" t="s">
-        <v>30</v>
+      <c r="I65" s="3">
+        <f t="shared" si="1"/>
+        <v>17</v>
       </c>
     </row>
     <row r="66">
@@ -2531,8 +2701,9 @@
       <c r="G66" s="2">
         <v>15.0</v>
       </c>
-      <c r="H66" s="2" t="s">
-        <v>30</v>
+      <c r="I66" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="67">
@@ -2557,8 +2728,9 @@
       <c r="G67" s="2">
         <v>13.0</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>30</v>
+      <c r="I67" s="3">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
       </c>
     </row>
     <row r="68">
@@ -2583,8 +2755,9 @@
       <c r="G68" s="2">
         <v>11.5</v>
       </c>
-      <c r="H68" s="2" t="s">
-        <v>30</v>
+      <c r="I68" s="3">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
       </c>
     </row>
     <row r="69">
@@ -2609,8 +2782,9 @@
       <c r="G69" s="2">
         <v>12.0</v>
       </c>
-      <c r="H69" s="2" t="s">
-        <v>30</v>
+      <c r="I69" s="3">
+        <f t="shared" si="1"/>
+        <v>11.5</v>
       </c>
     </row>
     <row r="70">
@@ -2635,8 +2809,9 @@
       <c r="G70" s="2">
         <v>119.0</v>
       </c>
-      <c r="H70" s="5" t="s">
-        <v>30</v>
+      <c r="I70" s="3">
+        <f t="shared" si="1"/>
+        <v>109</v>
       </c>
     </row>
     <row r="71">
@@ -2661,8 +2836,9 @@
       <c r="G71" s="2">
         <v>54.0</v>
       </c>
-      <c r="H71" s="2" t="s">
-        <v>30</v>
+      <c r="I71" s="3">
+        <f t="shared" si="1"/>
+        <v>47</v>
       </c>
     </row>
     <row r="72">
@@ -2687,8 +2863,9 @@
       <c r="G72" s="2">
         <v>35.0</v>
       </c>
-      <c r="H72" s="2" t="s">
-        <v>30</v>
+      <c r="I72" s="3">
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
     </row>
     <row r="73">
@@ -2713,8 +2890,9 @@
       <c r="G73" s="2">
         <v>27.0</v>
       </c>
-      <c r="H73" s="2" t="s">
-        <v>30</v>
+      <c r="I73" s="3">
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
     </row>
     <row r="74">
@@ -2739,8 +2917,9 @@
       <c r="G74" s="2">
         <v>21.0</v>
       </c>
-      <c r="H74" s="2" t="s">
-        <v>30</v>
+      <c r="I74" s="3">
+        <f t="shared" si="1"/>
+        <v>21</v>
       </c>
     </row>
     <row r="75">
@@ -2765,8 +2944,9 @@
       <c r="G75" s="2">
         <v>17.0</v>
       </c>
-      <c r="H75" s="2" t="s">
-        <v>30</v>
+      <c r="I75" s="3">
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
     </row>
     <row r="76">
@@ -2791,8 +2971,9 @@
       <c r="G76" s="2">
         <v>14.0</v>
       </c>
-      <c r="H76" s="2" t="s">
-        <v>30</v>
+      <c r="I76" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="77">
@@ -2817,8 +2998,9 @@
       <c r="G77" s="2">
         <v>15.5</v>
       </c>
-      <c r="H77" s="2" t="s">
-        <v>30</v>
+      <c r="I77" s="3">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
       </c>
     </row>
     <row r="78">
@@ -2843,8 +3025,9 @@
       <c r="G78" s="2">
         <v>11.0</v>
       </c>
-      <c r="H78" s="2" t="s">
-        <v>30</v>
+      <c r="I78" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
     </row>
     <row r="79">
@@ -2869,8 +3052,9 @@
       <c r="G79" s="2">
         <v>10.0</v>
       </c>
-      <c r="H79" s="2" t="s">
-        <v>30</v>
+      <c r="I79" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="80">
@@ -2878,7 +3062,7 @@
         <v>164</v>
       </c>
       <c r="B80" s="3" t="str">
-        <f t="shared" ref="B80:B119" si="2">"Day"&amp;C80&amp;"-"&amp;D80&amp;"-"&amp;E80&amp;"mms.mov"</f>
+        <f t="shared" ref="B80:B119" si="3">"Day"&amp;C80&amp;"-"&amp;D80&amp;"-"&amp;E80&amp;"mms.mov"</f>
         <v>Day8-Earth-1mms.mov</v>
       </c>
       <c r="C80" s="2">
@@ -2898,6 +3082,10 @@
       </c>
       <c r="H80" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="I80" s="3">
+        <f t="shared" si="1"/>
+        <v>124</v>
       </c>
     </row>
     <row r="81">
@@ -2905,7 +3093,7 @@
         <v>165</v>
       </c>
       <c r="B81" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day8-Earth-2mms.mov</v>
       </c>
       <c r="C81" s="2">
@@ -2922,6 +3110,10 @@
       </c>
       <c r="G81" s="2">
         <v>63.0</v>
+      </c>
+      <c r="I81" s="3">
+        <f t="shared" si="1"/>
+        <v>61</v>
       </c>
     </row>
     <row r="82">
@@ -2929,7 +3121,7 @@
         <v>166</v>
       </c>
       <c r="B82" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day8-Earth-3mms.mov</v>
       </c>
       <c r="C82" s="2">
@@ -2946,6 +3138,10 @@
       </c>
       <c r="G82" s="2">
         <v>41.0</v>
+      </c>
+      <c r="I82" s="3">
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
     </row>
     <row r="83">
@@ -2953,7 +3149,7 @@
         <v>167</v>
       </c>
       <c r="B83" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day8-Earth-4mms.mov</v>
       </c>
       <c r="C83" s="2">
@@ -2970,6 +3166,10 @@
       </c>
       <c r="G83" s="2">
         <v>30.0</v>
+      </c>
+      <c r="I83" s="3">
+        <f t="shared" si="1"/>
+        <v>28</v>
       </c>
     </row>
     <row r="84">
@@ -2977,7 +3177,7 @@
         <v>168</v>
       </c>
       <c r="B84" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day8-Earth-5mms.mov</v>
       </c>
       <c r="C84" s="2">
@@ -2994,6 +3194,10 @@
       </c>
       <c r="G84" s="2">
         <v>26.0</v>
+      </c>
+      <c r="I84" s="3">
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
     </row>
     <row r="85">
@@ -3001,7 +3205,7 @@
         <v>169</v>
       </c>
       <c r="B85" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day8-Earth-6mms.mov</v>
       </c>
       <c r="C85" s="2">
@@ -3018,6 +3222,10 @@
       </c>
       <c r="G85" s="2">
         <v>22.0</v>
+      </c>
+      <c r="I85" s="3">
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
     </row>
     <row r="86">
@@ -3025,7 +3233,7 @@
         <v>170</v>
       </c>
       <c r="B86" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day8-Earth-7mms.mov</v>
       </c>
       <c r="C86" s="2">
@@ -3042,6 +3250,10 @@
       </c>
       <c r="G86" s="2">
         <v>19.0</v>
+      </c>
+      <c r="I86" s="3">
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
     </row>
     <row r="87">
@@ -3049,7 +3261,7 @@
         <v>171</v>
       </c>
       <c r="B87" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day8-Earth-8mms.mov</v>
       </c>
       <c r="C87" s="2">
@@ -3066,6 +3278,10 @@
       </c>
       <c r="G87" s="2">
         <v>18.0</v>
+      </c>
+      <c r="I87" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="88">
@@ -3073,7 +3289,7 @@
         <v>172</v>
       </c>
       <c r="B88" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day8-Earth-9mms.mov</v>
       </c>
       <c r="C88" s="2">
@@ -3090,6 +3306,10 @@
       </c>
       <c r="G88" s="2">
         <v>16.0</v>
+      </c>
+      <c r="I88" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="89">
@@ -3097,7 +3317,7 @@
         <v>173</v>
       </c>
       <c r="B89" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day8-Earth-10mms.mov</v>
       </c>
       <c r="C89" s="2">
@@ -3114,6 +3334,10 @@
       </c>
       <c r="G89" s="2">
         <v>14.0</v>
+      </c>
+      <c r="I89" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
     </row>
     <row r="90">
@@ -3121,7 +3345,7 @@
         <v>174</v>
       </c>
       <c r="B90" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day9-Earth-1mms.mov</v>
       </c>
       <c r="C90" s="2">
@@ -3141,6 +3365,10 @@
       </c>
       <c r="H90" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="I90" s="3">
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
     </row>
     <row r="91">
@@ -3148,7 +3376,7 @@
         <v>175</v>
       </c>
       <c r="B91" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day9-Earth-2mms.mov</v>
       </c>
       <c r="C91" s="2">
@@ -3165,6 +3393,10 @@
       </c>
       <c r="G91" s="2">
         <v>62.0</v>
+      </c>
+      <c r="I91" s="3">
+        <f t="shared" si="1"/>
+        <v>60</v>
       </c>
     </row>
     <row r="92">
@@ -3172,7 +3404,7 @@
         <v>176</v>
       </c>
       <c r="B92" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day9-Earth-3mms.mov</v>
       </c>
       <c r="C92" s="2">
@@ -3189,6 +3421,10 @@
       </c>
       <c r="G92" s="2">
         <v>40.0</v>
+      </c>
+      <c r="I92" s="3">
+        <f t="shared" si="1"/>
+        <v>39</v>
       </c>
     </row>
     <row r="93">
@@ -3196,7 +3432,7 @@
         <v>177</v>
       </c>
       <c r="B93" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day9-Earth-4mms.mov</v>
       </c>
       <c r="C93" s="2">
@@ -3213,6 +3449,10 @@
       </c>
       <c r="G93" s="2">
         <v>33.0</v>
+      </c>
+      <c r="I93" s="3">
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
     </row>
     <row r="94">
@@ -3220,7 +3460,7 @@
         <v>178</v>
       </c>
       <c r="B94" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day9-Earth-5mms.mov</v>
       </c>
       <c r="C94" s="2">
@@ -3237,6 +3477,10 @@
       </c>
       <c r="G94" s="2">
         <v>26.0</v>
+      </c>
+      <c r="I94" s="3">
+        <f t="shared" si="1"/>
+        <v>24</v>
       </c>
     </row>
     <row r="95">
@@ -3244,7 +3488,7 @@
         <v>179</v>
       </c>
       <c r="B95" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day9-Earth-6mms.mov</v>
       </c>
       <c r="C95" s="2">
@@ -3261,6 +3505,10 @@
       </c>
       <c r="G95" s="2">
         <v>22.0</v>
+      </c>
+      <c r="I95" s="3">
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
     </row>
     <row r="96">
@@ -3268,7 +3516,7 @@
         <v>180</v>
       </c>
       <c r="B96" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day9-Earth-7mms.mov</v>
       </c>
       <c r="C96" s="2">
@@ -3285,6 +3533,10 @@
       </c>
       <c r="G96" s="2">
         <v>19.0</v>
+      </c>
+      <c r="I96" s="3">
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
     </row>
     <row r="97">
@@ -3292,7 +3544,7 @@
         <v>181</v>
       </c>
       <c r="B97" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day9-Earth-8mms.mov</v>
       </c>
       <c r="C97" s="2">
@@ -3304,11 +3556,15 @@
       <c r="E97" s="2">
         <v>8.0</v>
       </c>
-      <c r="F97" s="5">
+      <c r="F97" s="2">
         <v>2.0</v>
       </c>
       <c r="G97" s="2">
         <v>17.0</v>
+      </c>
+      <c r="I97" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="98">
@@ -3316,7 +3572,7 @@
         <v>182</v>
       </c>
       <c r="B98" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day9-Earth-9mms.mov</v>
       </c>
       <c r="C98" s="2">
@@ -3331,8 +3587,12 @@
       <c r="F98" s="2">
         <v>1.5</v>
       </c>
-      <c r="G98" s="5">
+      <c r="G98" s="2">
         <v>16.0</v>
+      </c>
+      <c r="I98" s="3">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
       </c>
     </row>
     <row r="99">
@@ -3340,7 +3600,7 @@
         <v>183</v>
       </c>
       <c r="B99" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day9-Earth-10mms.mov</v>
       </c>
       <c r="C99" s="2">
@@ -3357,6 +3617,10 @@
       </c>
       <c r="G99" s="2">
         <v>13.5</v>
+      </c>
+      <c r="I99" s="3">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
       </c>
     </row>
     <row r="100">
@@ -3364,7 +3628,7 @@
         <v>184</v>
       </c>
       <c r="B100" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day10-Earth-1mms.mov</v>
       </c>
       <c r="C100" s="2">
@@ -3384,6 +3648,10 @@
       </c>
       <c r="H100" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="I100" s="3">
+        <f t="shared" si="1"/>
+        <v>134</v>
       </c>
     </row>
     <row r="101">
@@ -3391,7 +3659,7 @@
         <v>185</v>
       </c>
       <c r="B101" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day10-Earth-2mms.mov</v>
       </c>
       <c r="C101" s="2">
@@ -3408,6 +3676,10 @@
       </c>
       <c r="G101" s="2">
         <v>65.0</v>
+      </c>
+      <c r="I101" s="3">
+        <f t="shared" si="1"/>
+        <v>64</v>
       </c>
     </row>
     <row r="102">
@@ -3415,7 +3687,7 @@
         <v>186</v>
       </c>
       <c r="B102" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day10-Earth-3mms.mov</v>
       </c>
       <c r="C102" s="2">
@@ -3432,6 +3704,10 @@
       </c>
       <c r="G102" s="2">
         <v>43.0</v>
+      </c>
+      <c r="I102" s="3">
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
     </row>
     <row r="103">
@@ -3439,7 +3715,7 @@
         <v>187</v>
       </c>
       <c r="B103" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day10-Earth-4mms.mov</v>
       </c>
       <c r="C103" s="2">
@@ -3456,6 +3732,10 @@
       </c>
       <c r="G103" s="2">
         <v>35.0</v>
+      </c>
+      <c r="I103" s="3">
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
     </row>
     <row r="104">
@@ -3463,7 +3743,7 @@
         <v>188</v>
       </c>
       <c r="B104" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day10-Earth-5mms.mov</v>
       </c>
       <c r="C104" s="2">
@@ -3480,6 +3760,10 @@
       </c>
       <c r="G104" s="2">
         <v>28.0</v>
+      </c>
+      <c r="I104" s="3">
+        <f t="shared" si="1"/>
+        <v>25.5</v>
       </c>
     </row>
     <row r="105">
@@ -3487,7 +3771,7 @@
         <v>189</v>
       </c>
       <c r="B105" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day10-Earth-6mms.mov</v>
       </c>
       <c r="C105" s="2">
@@ -3504,6 +3788,10 @@
       </c>
       <c r="G105" s="2">
         <v>22.0</v>
+      </c>
+      <c r="I105" s="3">
+        <f t="shared" si="1"/>
+        <v>20.5</v>
       </c>
     </row>
     <row r="106">
@@ -3511,7 +3799,7 @@
         <v>190</v>
       </c>
       <c r="B106" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day10-Earth-7mms.mov</v>
       </c>
       <c r="C106" s="2">
@@ -3528,6 +3816,10 @@
       </c>
       <c r="G106" s="2">
         <v>20.0</v>
+      </c>
+      <c r="I106" s="3">
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
     </row>
     <row r="107">
@@ -3535,7 +3827,7 @@
         <v>191</v>
       </c>
       <c r="B107" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day10-Earth-8mms.mov</v>
       </c>
       <c r="C107" s="2">
@@ -3552,6 +3844,10 @@
       </c>
       <c r="G107" s="2">
         <v>17.0</v>
+      </c>
+      <c r="I107" s="3">
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
     </row>
     <row r="108">
@@ -3559,7 +3855,7 @@
         <v>192</v>
       </c>
       <c r="B108" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day10-Earth-9mms.mov</v>
       </c>
       <c r="C108" s="2">
@@ -3576,6 +3872,10 @@
       </c>
       <c r="G108" s="2">
         <v>15.0</v>
+      </c>
+      <c r="I108" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="109">
@@ -3583,7 +3883,7 @@
         <v>193</v>
       </c>
       <c r="B109" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day10-Earth-10mms.mov</v>
       </c>
       <c r="C109" s="2">
@@ -3600,6 +3900,10 @@
       </c>
       <c r="G109" s="2">
         <v>13.0</v>
+      </c>
+      <c r="I109" s="3">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
       </c>
     </row>
     <row r="110">
@@ -3607,7 +3911,7 @@
         <v>194</v>
       </c>
       <c r="B110" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day11-Earth-1mms.mov</v>
       </c>
       <c r="C110" s="2">
@@ -3627,6 +3931,10 @@
       </c>
       <c r="H110" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="I110" s="3">
+        <f t="shared" si="1"/>
+        <v>138</v>
       </c>
     </row>
     <row r="111">
@@ -3634,7 +3942,7 @@
         <v>195</v>
       </c>
       <c r="B111" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day11-Earth-2mms.mov</v>
       </c>
       <c r="C111" s="2">
@@ -3651,6 +3959,10 @@
       </c>
       <c r="G111" s="2">
         <v>67.0</v>
+      </c>
+      <c r="I111" s="3">
+        <f t="shared" si="1"/>
+        <v>65</v>
       </c>
     </row>
     <row r="112">
@@ -3658,7 +3970,7 @@
         <v>196</v>
       </c>
       <c r="B112" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day11-Earth-3mms.mov</v>
       </c>
       <c r="C112" s="2">
@@ -3675,6 +3987,10 @@
       </c>
       <c r="G112" s="2">
         <v>44.0</v>
+      </c>
+      <c r="I112" s="3">
+        <f t="shared" si="1"/>
+        <v>42.5</v>
       </c>
     </row>
     <row r="113">
@@ -3682,7 +3998,7 @@
         <v>197</v>
       </c>
       <c r="B113" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day11-Earth-4mms.mov</v>
       </c>
       <c r="C113" s="2">
@@ -3699,6 +4015,10 @@
       </c>
       <c r="G113" s="2">
         <v>33.0</v>
+      </c>
+      <c r="I113" s="3">
+        <f t="shared" si="1"/>
+        <v>32</v>
       </c>
     </row>
     <row r="114">
@@ -3706,7 +4026,7 @@
         <v>198</v>
       </c>
       <c r="B114" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day11-Earth-5mms.mov</v>
       </c>
       <c r="C114" s="2">
@@ -3723,6 +4043,10 @@
       </c>
       <c r="G114" s="2">
         <v>26.0</v>
+      </c>
+      <c r="I114" s="3">
+        <f t="shared" si="1"/>
+        <v>24.5</v>
       </c>
     </row>
     <row r="115">
@@ -3730,7 +4054,7 @@
         <v>199</v>
       </c>
       <c r="B115" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day11-Earth-6mms.mov</v>
       </c>
       <c r="C115" s="2">
@@ -3747,6 +4071,10 @@
       </c>
       <c r="G115" s="2">
         <v>22.0</v>
+      </c>
+      <c r="I115" s="3">
+        <f t="shared" si="1"/>
+        <v>21</v>
       </c>
     </row>
     <row r="116">
@@ -3754,7 +4082,7 @@
         <v>200</v>
       </c>
       <c r="B116" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day11-Earth-7mms.mov</v>
       </c>
       <c r="C116" s="2">
@@ -3771,6 +4099,10 @@
       </c>
       <c r="G116" s="2">
         <v>19.0</v>
+      </c>
+      <c r="I116" s="3">
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
     </row>
     <row r="117">
@@ -3778,7 +4110,7 @@
         <v>201</v>
       </c>
       <c r="B117" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day11-Earth-8mms.mov</v>
       </c>
       <c r="C117" s="2">
@@ -3795,6 +4127,10 @@
       </c>
       <c r="G117" s="2">
         <v>17.0</v>
+      </c>
+      <c r="I117" s="3">
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
     </row>
     <row r="118">
@@ -3802,7 +4138,7 @@
         <v>202</v>
       </c>
       <c r="B118" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day11-Earth-9mms.mov</v>
       </c>
       <c r="C118" s="2">
@@ -3819,6 +4155,10 @@
       </c>
       <c r="G118" s="2">
         <v>15.5</v>
+      </c>
+      <c r="I118" s="3">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
       </c>
     </row>
     <row r="119">
@@ -3826,7 +4166,7 @@
         <v>203</v>
       </c>
       <c r="B119" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Day11-Earth-10mms.mov</v>
       </c>
       <c r="C119" s="2">
@@ -3843,6 +4183,14 @@
       </c>
       <c r="G119" s="2">
         <v>14.0</v>
+      </c>
+      <c r="I119" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J119" s="3">
+        <f>sum(I3:I119) / 60</f>
+        <v>54.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>